<commit_message>
Planilha de análise de fatura
</commit_message>
<xml_diff>
--- a/arquivos/Teste.xlsx
+++ b/arquivos/Teste.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
-    <sheet name="Análise" sheetId="2" r:id="rId2"/>
+    <sheet name="Comparativo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>DEZ/23</t>
   </si>
@@ -102,13 +102,66 @@
   </si>
   <si>
     <t>Custo Demanda Reativa</t>
+  </si>
+  <si>
+    <t>MÊS/ANO</t>
+  </si>
+  <si>
+    <t>DEMANDA</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>R$</t>
+  </si>
+  <si>
+    <t>ULTRAPASSAGEM</t>
+  </si>
+  <si>
+    <t>CONSUMO</t>
+  </si>
+  <si>
+    <t>PONTA</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>FORA DE PONTA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Demanda Contratada P Atual:</t>
+  </si>
+  <si>
+    <t>Demanda Contratada FP Atual:</t>
+  </si>
+  <si>
+    <t>Demanda Contratada P Recomendada:</t>
+  </si>
+  <si>
+    <t>Demanda Contratada FP Recomendada:</t>
+  </si>
+  <si>
+    <t>Custo - Verde</t>
+  </si>
+  <si>
+    <t>Custo - Azul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="#,##0.00 &quot;kW&quot;"/>
+    <numFmt numFmtId="165" formatCode="R$ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00 &quot;kWh&quot;"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,16 +169,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,12 +225,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,6 +298,290 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Verde</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparativo'!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN/23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEV/23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR/23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ABR/23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAI/23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN/23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL/23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AGO/23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SET/23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OUT/23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV/23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEZ/23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparativo'!$J$4:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>53140.07998734999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55086.30186711</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49586.23364305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55506.98194519</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52203.70853644</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56061.31273675</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55716.93268549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57985.01330517</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59765.05869915</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63440.23088899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60509.37502902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57678.02190802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Azul</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparativo'!$Y$4:$Y$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>52280.7708684</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53284.02397394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49815.18206370001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53292.08245626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52482.73257576</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53849.5676175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53419.23099246</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56080.0023798</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56160.84712628</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59910.65219158</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>57597.84625278</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55329.24538833999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Custo Mensal Estimado (R$)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln w="15875">
+      <a:solidFill>
+        <a:srgbClr val="4472C4"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,7 +1005,7 @@
         <v>7389.16</v>
       </c>
       <c r="K2">
-        <v>18757.99596028</v>
+        <v>4884.101755119999</v>
       </c>
       <c r="L2">
         <v>53340</v>
@@ -622,7 +1058,7 @@
         <v>7636.86</v>
       </c>
       <c r="K3">
-        <v>19386.80296938</v>
+        <v>5047.82699652</v>
       </c>
       <c r="L3">
         <v>55377</v>
@@ -675,7 +1111,7 @@
         <v>7966.03</v>
       </c>
       <c r="K4">
-        <v>20222.42833549</v>
+        <v>5265.40244146</v>
       </c>
       <c r="L4">
         <v>59052</v>
@@ -728,7 +1164,7 @@
         <v>7905.87</v>
       </c>
       <c r="K5">
-        <v>20069.70718221</v>
+        <v>5225.637764339999</v>
       </c>
       <c r="L5">
         <v>54316.5</v>
@@ -781,7 +1217,7 @@
         <v>7274.19</v>
       </c>
       <c r="K6">
-        <v>18466.13507277</v>
+        <v>4808.108654579999</v>
       </c>
       <c r="L6">
         <v>54022.5</v>
@@ -834,7 +1270,7 @@
         <v>7210.03</v>
       </c>
       <c r="K7">
-        <v>18303.25958749</v>
+        <v>4765.70004946</v>
       </c>
       <c r="L7">
         <v>51303</v>
@@ -887,7 +1323,7 @@
         <v>7164.25</v>
       </c>
       <c r="K8">
-        <v>18187.04325775</v>
+        <v>4735.4402935</v>
       </c>
       <c r="L8">
         <v>52395</v>
@@ -940,7 +1376,7 @@
         <v>5837.68</v>
       </c>
       <c r="K9">
-        <v>14819.43520744</v>
+        <v>3858.60140176</v>
       </c>
       <c r="L9">
         <v>51639</v>
@@ -993,7 +1429,7 @@
         <v>7165.93</v>
       </c>
       <c r="K10">
-        <v>18191.30807719</v>
+        <v>4736.55074326</v>
       </c>
       <c r="L10">
         <v>51418.5</v>
@@ -1046,7 +1482,7 @@
         <v>5864.35</v>
       </c>
       <c r="K11">
-        <v>14887.13921605</v>
+        <v>3876.2297917</v>
       </c>
       <c r="L11">
         <v>47302.5</v>
@@ -1099,7 +1535,7 @@
         <v>6946.17</v>
       </c>
       <c r="K12">
-        <v>17633.42907711</v>
+        <v>4591.29333894</v>
       </c>
       <c r="L12">
         <v>51303</v>
@@ -1152,7 +1588,7 @@
         <v>6443.95</v>
       </c>
       <c r="K13">
-        <v>16358.50192285</v>
+        <v>4259.3349589</v>
       </c>
       <c r="L13">
         <v>50095.5</v>
@@ -1183,811 +1619,1116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:V13"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="14.7109375" customWidth="1"/>
+    <col min="12" max="25" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22">
-      <c r="A2" t="s">
+    <row r="1" spans="1:25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B4" s="3">
         <v>140.28</v>
       </c>
-      <c r="C2">
+      <c r="C4" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>6443.95</v>
       </c>
-      <c r="F2">
+      <c r="G4" s="4">
         <v>16358.50192285</v>
       </c>
-      <c r="G2">
+      <c r="H4" s="5">
         <v>50095.5</v>
       </c>
-      <c r="H2">
+      <c r="I4" s="4">
         <v>31962.4488645</v>
       </c>
-      <c r="I2">
+      <c r="J4" s="4">
         <v>53140.07998734999</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2">
+      <c r="M4" s="6">
         <v>122.22</v>
       </c>
-      <c r="M2">
+      <c r="N4" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
         <v>140.28</v>
       </c>
-      <c r="P2">
+      <c r="R4" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7">
+        <v>0</v>
+      </c>
+      <c r="U4" s="8">
         <v>6443.95</v>
       </c>
-      <c r="S2">
-        <v>16358.50192285</v>
-      </c>
-      <c r="T2">
+      <c r="V4" s="7">
+        <v>4259.3349589</v>
+      </c>
+      <c r="W4" s="8">
         <v>50095.5</v>
       </c>
-      <c r="U2">
+      <c r="X4" s="7">
         <v>31962.4488645</v>
       </c>
-      <c r="V2">
-        <v>64379.93783235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
+      <c r="Y4" s="7">
+        <v>52280.7708684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B5" s="3">
         <v>137.76</v>
       </c>
-      <c r="C3">
+      <c r="C5" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
         <v>6946.17</v>
       </c>
-      <c r="F3">
+      <c r="G5" s="4">
         <v>17633.42907711</v>
       </c>
-      <c r="G3">
+      <c r="H5" s="5">
         <v>51303</v>
       </c>
-      <c r="H3">
+      <c r="I5" s="4">
         <v>32633.74359</v>
       </c>
-      <c r="I3">
+      <c r="J5" s="4">
         <v>55086.30186711</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3">
+      <c r="M5" s="6">
         <v>129.78</v>
       </c>
-      <c r="M3">
+      <c r="N5" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
         <v>137.76</v>
       </c>
-      <c r="P3">
+      <c r="R5" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7">
+        <v>0</v>
+      </c>
+      <c r="U5" s="8">
         <v>6946.17</v>
       </c>
-      <c r="S3">
-        <v>17633.42907711</v>
-      </c>
-      <c r="T3">
+      <c r="V5" s="7">
+        <v>4591.29333894</v>
+      </c>
+      <c r="W5" s="8">
         <v>51303</v>
       </c>
-      <c r="U3">
+      <c r="X5" s="7">
         <v>32633.74359</v>
       </c>
-      <c r="V3">
-        <v>66326.15971211001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
+      <c r="Y5" s="7">
+        <v>53284.02397394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B6" s="3">
         <v>142.8</v>
       </c>
-      <c r="C4">
+      <c r="C6" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
         <v>5864.35</v>
       </c>
-      <c r="F4">
+      <c r="G6" s="4">
         <v>14887.13921605</v>
       </c>
-      <c r="G4">
+      <c r="H6" s="5">
         <v>47302.5</v>
       </c>
-      <c r="H4">
+      <c r="I6" s="4">
         <v>29879.965227</v>
       </c>
-      <c r="I4">
+      <c r="J6" s="4">
         <v>49586.23364305</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L4">
+      <c r="M6" s="6">
         <v>127.26</v>
       </c>
-      <c r="M4">
+      <c r="N6" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="O6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="6">
         <v>142.8</v>
       </c>
-      <c r="P4">
+      <c r="R6" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7">
+        <v>0</v>
+      </c>
+      <c r="U6" s="8">
         <v>5864.35</v>
       </c>
-      <c r="S4">
-        <v>14887.13921605</v>
-      </c>
-      <c r="T4">
+      <c r="V6" s="7">
+        <v>3876.2297917</v>
+      </c>
+      <c r="W6" s="8">
         <v>47302.5</v>
       </c>
-      <c r="U4">
+      <c r="X6" s="7">
         <v>29879.965227</v>
       </c>
-      <c r="V4">
-        <v>60826.09148805001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
+      <c r="Y6" s="7">
+        <v>49815.18206370001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B7" s="3">
         <v>136.08</v>
       </c>
-      <c r="C5">
+      <c r="C7" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
         <v>7165.93</v>
       </c>
-      <c r="F5">
+      <c r="G7" s="4">
         <v>18191.30807719</v>
       </c>
-      <c r="G5">
+      <c r="H7" s="5">
         <v>51418.5</v>
       </c>
-      <c r="H5">
+      <c r="I7" s="4">
         <v>32496.544668</v>
       </c>
-      <c r="I5">
+      <c r="J7" s="4">
         <v>55506.98194519</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L5">
+      <c r="M7" s="6">
         <v>124.32</v>
       </c>
-      <c r="M5">
+      <c r="N7" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
+      <c r="O7" s="6">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="6">
         <v>136.08</v>
       </c>
-      <c r="P5">
+      <c r="R7" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
+      <c r="S7" s="6">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="8">
         <v>7165.93</v>
       </c>
-      <c r="S5">
-        <v>18191.30807719</v>
-      </c>
-      <c r="T5">
+      <c r="V7" s="7">
+        <v>4736.55074326</v>
+      </c>
+      <c r="W7" s="8">
         <v>51418.5</v>
       </c>
-      <c r="U5">
+      <c r="X7" s="7">
         <v>32496.544668</v>
       </c>
-      <c r="V5">
-        <v>66746.83979019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
+      <c r="Y7" s="7">
+        <v>53292.08245626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B8" s="3">
         <v>138.6</v>
       </c>
-      <c r="C6">
+      <c r="C8" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
         <v>5837.68</v>
       </c>
-      <c r="F6">
+      <c r="G8" s="4">
         <v>14819.43520744</v>
       </c>
-      <c r="G6">
+      <c r="H8" s="5">
         <v>51639</v>
       </c>
-      <c r="H6">
+      <c r="I8" s="4">
         <v>32565.144129</v>
       </c>
-      <c r="I6">
+      <c r="J8" s="4">
         <v>52203.70853644</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L6">
+      <c r="M8" s="6">
         <v>126</v>
       </c>
-      <c r="M6">
+      <c r="N8" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
+      <c r="O8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="6">
         <v>138.6</v>
       </c>
-      <c r="P6">
+      <c r="R8" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
+      <c r="S8" s="6">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7">
+        <v>0</v>
+      </c>
+      <c r="U8" s="8">
         <v>5837.68</v>
       </c>
-      <c r="S6">
-        <v>14819.43520744</v>
-      </c>
-      <c r="T6">
+      <c r="V8" s="7">
+        <v>3858.60140176</v>
+      </c>
+      <c r="W8" s="8">
         <v>51639</v>
       </c>
-      <c r="U6">
+      <c r="X8" s="7">
         <v>32565.144129</v>
       </c>
-      <c r="V6">
-        <v>63443.56638144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" t="s">
+      <c r="Y8" s="7">
+        <v>52482.73257576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B9" s="3">
         <v>132.72</v>
       </c>
-      <c r="C7">
+      <c r="C9" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
         <v>7164.25</v>
       </c>
-      <c r="F7">
+      <c r="G9" s="4">
         <v>18187.04325775</v>
       </c>
-      <c r="G7">
+      <c r="H9" s="5">
         <v>52395</v>
       </c>
-      <c r="H7">
+      <c r="I9" s="4">
         <v>33055.140279</v>
       </c>
-      <c r="I7">
+      <c r="J9" s="4">
         <v>56061.31273675</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L7">
+      <c r="M9" s="6">
         <v>123.9</v>
       </c>
-      <c r="M7">
+      <c r="N9" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
+      <c r="O9" s="6">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6">
         <v>132.72</v>
       </c>
-      <c r="P7">
+      <c r="R9" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
+      <c r="S9" s="6">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7">
+        <v>0</v>
+      </c>
+      <c r="U9" s="8">
         <v>7164.25</v>
       </c>
-      <c r="S7">
-        <v>18187.04325775</v>
-      </c>
-      <c r="T7">
+      <c r="V9" s="7">
+        <v>4735.4402935</v>
+      </c>
+      <c r="W9" s="8">
         <v>52395</v>
       </c>
-      <c r="U7">
+      <c r="X9" s="7">
         <v>33055.140279</v>
       </c>
-      <c r="V7">
-        <v>67301.17058174999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" t="s">
+      <c r="Y9" s="7">
+        <v>53849.5676175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B10" s="3">
         <v>137.76</v>
       </c>
-      <c r="C8">
+      <c r="C10" s="4">
         <v>4819.129199999999</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
         <v>7210.03</v>
       </c>
-      <c r="F8">
+      <c r="G10" s="4">
         <v>18303.25958749</v>
       </c>
-      <c r="G8">
+      <c r="H10" s="5">
         <v>51303</v>
       </c>
-      <c r="H8">
+      <c r="I10" s="4">
         <v>32594.543898</v>
       </c>
-      <c r="I8">
+      <c r="J10" s="4">
         <v>55716.93268549</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L8">
+      <c r="M10" s="6">
         <v>124.74</v>
       </c>
-      <c r="M8">
+      <c r="N10" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
         <v>137.76</v>
       </c>
-      <c r="P8">
+      <c r="R10" s="7">
         <v>4819.129199999999</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
+      <c r="S10" s="6">
+        <v>0</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0</v>
+      </c>
+      <c r="U10" s="8">
         <v>7210.03</v>
       </c>
-      <c r="S8">
-        <v>18303.25958749</v>
-      </c>
-      <c r="T8">
+      <c r="V10" s="7">
+        <v>4765.70004946</v>
+      </c>
+      <c r="W10" s="8">
         <v>51303</v>
       </c>
-      <c r="U8">
+      <c r="X10" s="7">
         <v>32594.543898</v>
       </c>
-      <c r="V8">
-        <v>66956.79053049001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" t="s">
+      <c r="Y10" s="7">
+        <v>53419.23099246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B11" s="3">
         <v>153.3</v>
       </c>
-      <c r="C9">
+      <c r="C11" s="4">
         <v>4925.1500424</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
         <v>7274.19</v>
       </c>
-      <c r="F9">
+      <c r="G11" s="4">
         <v>18466.13507277</v>
       </c>
-      <c r="G9">
+      <c r="H11" s="5">
         <v>54022.5</v>
       </c>
-      <c r="H9">
+      <c r="I11" s="4">
         <v>34593.72819</v>
       </c>
-      <c r="I9">
+      <c r="J11" s="4">
         <v>57985.01330517</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L9">
+      <c r="M11" s="6">
         <v>151.62</v>
       </c>
-      <c r="M9">
+      <c r="N11" s="7">
         <v>11753.01549282</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
+      <c r="O11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
         <v>153.3</v>
       </c>
-      <c r="P9">
+      <c r="R11" s="7">
         <v>4925.1500424</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
+      <c r="S11" s="6">
+        <v>0</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0</v>
+      </c>
+      <c r="U11" s="8">
         <v>7274.19</v>
       </c>
-      <c r="S9">
-        <v>18466.13507277</v>
-      </c>
-      <c r="T9">
+      <c r="V11" s="7">
+        <v>4808.108654579999</v>
+      </c>
+      <c r="W11" s="8">
         <v>54022.5</v>
       </c>
-      <c r="U9">
+      <c r="X11" s="7">
         <v>34593.72819</v>
       </c>
-      <c r="V9">
-        <v>69738.02879799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" t="s">
+      <c r="Y11" s="7">
+        <v>56080.0023798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B10">
+      <c r="B12" s="3">
         <v>154.98</v>
       </c>
-      <c r="C10">
+      <c r="C12" s="4">
         <v>4979.124289439999</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
         <v>7905.87</v>
       </c>
-      <c r="F10">
+      <c r="G12" s="4">
         <v>20069.70718221</v>
       </c>
-      <c r="G10">
+      <c r="H12" s="5">
         <v>54316.5</v>
       </c>
-      <c r="H10">
+      <c r="I12" s="4">
         <v>34716.2272275</v>
       </c>
-      <c r="I10">
+      <c r="J12" s="4">
         <v>59765.05869915</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L10">
+      <c r="M12" s="6">
         <v>140.7</v>
       </c>
-      <c r="M10">
+      <c r="N12" s="7">
         <v>11239.857845</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
+      <c r="O12" s="6">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
         <v>154.98</v>
       </c>
-      <c r="P10">
+      <c r="R12" s="7">
         <v>4979.124289439999</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
+      <c r="S12" s="6">
+        <v>0</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0</v>
+      </c>
+      <c r="U12" s="8">
         <v>7905.87</v>
       </c>
-      <c r="S10">
-        <v>20069.70718221</v>
-      </c>
-      <c r="T10">
+      <c r="V12" s="7">
+        <v>5225.637764339999</v>
+      </c>
+      <c r="W12" s="8">
         <v>54316.5</v>
       </c>
-      <c r="U10">
+      <c r="X12" s="7">
         <v>34716.2272275</v>
       </c>
-      <c r="V10">
-        <v>71004.91654415001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" t="s">
+      <c r="Y12" s="7">
+        <v>56160.84712628</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B13" s="3">
         <v>157.5</v>
       </c>
-      <c r="C11">
+      <c r="C13" s="4">
         <v>5060.08566</v>
       </c>
-      <c r="D11">
+      <c r="D13" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="E13" s="4">
         <v>481.91292</v>
       </c>
-      <c r="E11">
+      <c r="F13" s="5">
         <v>7966.03</v>
       </c>
-      <c r="F11">
+      <c r="G13" s="4">
         <v>20222.42833549</v>
       </c>
-      <c r="G11">
+      <c r="H13" s="5">
         <v>59052</v>
       </c>
-      <c r="H11">
+      <c r="I13" s="4">
         <v>37675.8039735</v>
       </c>
-      <c r="I11">
+      <c r="J13" s="4">
         <v>63440.23088899</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L11">
+      <c r="M13" s="6">
         <v>147.42</v>
       </c>
-      <c r="M11">
+      <c r="N13" s="7">
         <v>11427.44719662</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
         <v>157.5</v>
       </c>
-      <c r="P11">
+      <c r="R13" s="7">
         <v>5060.08566</v>
       </c>
-      <c r="Q11">
+      <c r="S13" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="T13" s="7">
         <v>481.91292</v>
       </c>
-      <c r="R11">
+      <c r="U13" s="8">
         <v>7966.03</v>
       </c>
-      <c r="S11">
-        <v>20222.42833549</v>
-      </c>
-      <c r="T11">
+      <c r="V13" s="7">
+        <v>5265.40244146</v>
+      </c>
+      <c r="W13" s="8">
         <v>59052</v>
       </c>
-      <c r="U11">
+      <c r="X13" s="7">
         <v>37675.8039735</v>
       </c>
-      <c r="V11">
-        <v>74867.67808561001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" t="s">
+      <c r="Y13" s="7">
+        <v>59910.65219158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B14" s="3">
         <v>162.96</v>
       </c>
-      <c r="C12">
+      <c r="C14" s="4">
         <v>5235.50196288</v>
       </c>
-      <c r="D12">
+      <c r="D14" s="3">
+        <v>12.96000000000001</v>
+      </c>
+      <c r="E14" s="4">
         <v>832.7455257600004</v>
       </c>
-      <c r="E12">
+      <c r="F14" s="5">
         <v>7636.86</v>
       </c>
-      <c r="F12">
+      <c r="G14" s="4">
         <v>19386.80296938</v>
       </c>
-      <c r="G12">
+      <c r="H14" s="5">
         <v>55377</v>
       </c>
-      <c r="H12">
+      <c r="I14" s="4">
         <v>35054.324571</v>
       </c>
-      <c r="I12">
+      <c r="J14" s="4">
         <v>60509.37502902</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L12">
+      <c r="M14" s="6">
         <v>147.42</v>
       </c>
-      <c r="M12">
+      <c r="N14" s="7">
         <v>11427.44719662</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
+      <c r="O14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6">
         <v>162.96</v>
       </c>
-      <c r="P12">
+      <c r="R14" s="7">
         <v>5235.50196288</v>
       </c>
-      <c r="Q12">
+      <c r="S14" s="6">
+        <v>12.96000000000001</v>
+      </c>
+      <c r="T14" s="7">
         <v>832.7455257600004</v>
       </c>
-      <c r="R12">
+      <c r="U14" s="8">
         <v>7636.86</v>
       </c>
-      <c r="S12">
-        <v>19386.80296938</v>
-      </c>
-      <c r="T12">
+      <c r="V14" s="7">
+        <v>5047.82699652</v>
+      </c>
+      <c r="W14" s="8">
         <v>55377</v>
       </c>
-      <c r="U12">
+      <c r="X14" s="7">
         <v>35054.324571</v>
       </c>
-      <c r="V12">
-        <v>71936.82222564</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
+      <c r="Y14" s="7">
+        <v>57597.84625278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3">
         <v>157.08</v>
       </c>
-      <c r="C13">
+      <c r="C15" s="4">
         <v>5046.59209824</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
         <v>7389.16</v>
       </c>
-      <c r="F13">
+      <c r="G15" s="4">
         <v>18757.99596028</v>
       </c>
-      <c r="G13">
+      <c r="H15" s="5">
         <v>53340</v>
       </c>
-      <c r="H13">
+      <c r="I15" s="4">
         <v>33873.4338495</v>
       </c>
-      <c r="I13">
+      <c r="J15" s="4">
         <v>57678.02190802</v>
       </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="L15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="6">
         <v>148.68</v>
       </c>
-      <c r="M13">
+      <c r="N15" s="7">
         <v>11525.11768548</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
+      <c r="O15" s="6">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6">
         <v>157.08</v>
       </c>
-      <c r="P13">
+      <c r="R15" s="7">
         <v>5046.59209824</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
+      <c r="S15" s="6">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7">
+        <v>0</v>
+      </c>
+      <c r="U15" s="8">
         <v>7389.16</v>
       </c>
-      <c r="S13">
-        <v>18757.99596028</v>
-      </c>
-      <c r="T13">
+      <c r="V15" s="7">
+        <v>4884.101755119999</v>
+      </c>
+      <c r="W15" s="8">
         <v>53340</v>
       </c>
-      <c r="U13">
+      <c r="X15" s="7">
         <v>33873.4338495</v>
       </c>
-      <c r="V13">
-        <v>69203.1395935</v>
+      <c r="Y15" s="7">
+        <v>55329.24538833999</v>
+      </c>
+    </row>
+    <row r="18" spans="13:18">
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="9">
+        <v>153</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="10">
+        <v>676679.25123173</v>
+      </c>
+    </row>
+    <row r="19" spans="13:18">
+      <c r="M19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="9">
+        <v>153</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R19" s="10">
+        <v>653502.1838868</v>
+      </c>
+    </row>
+    <row r="21" spans="13:18">
+      <c r="M21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" s="9">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="13:18">
+      <c r="M23" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="9">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:P2"/>
+    <mergeCell ref="Q1:T2"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
custo com demanda atual - análise por fatura
</commit_message>
<xml_diff>
--- a/arquivos/Teste.xlsx
+++ b/arquivos/Teste.xlsx
@@ -16,19 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
-  <si>
-    <t>JAN/23</t>
-  </si>
-  <si>
-    <t>FEV/23</t>
-  </si>
-  <si>
-    <t>MAR/23</t>
-  </si>
-  <si>
-    <t>ABR/23</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>MAI/23</t>
   </si>
@@ -54,31 +42,34 @@
     <t>DEZ/23</t>
   </si>
   <si>
+    <t>JAN/24</t>
+  </si>
+  <si>
+    <t>FEV/24</t>
+  </si>
+  <si>
+    <t>MAR/24</t>
+  </si>
+  <si>
+    <t>ABR/24</t>
+  </si>
+  <si>
     <t>Mês</t>
   </si>
   <si>
     <t>Demanda Registrada HP</t>
   </si>
   <si>
-    <t>Custo Demanda HP</t>
-  </si>
-  <si>
     <t>Demanda Registrada HFP</t>
   </si>
   <si>
-    <t>Custo Demanda HFP</t>
-  </si>
-  <si>
-    <t>Ultrapassagem Registrada HP</t>
-  </si>
-  <si>
-    <t>Custo Ultrapassagem HP</t>
-  </si>
-  <si>
-    <t>Ultrapassagem Registrada HFP</t>
-  </si>
-  <si>
-    <t>Custo Ultrapassagem HFP</t>
+    <t>Custo Demanda</t>
+  </si>
+  <si>
+    <t>Ultrapassagem Registrada</t>
+  </si>
+  <si>
+    <t>Custo Ultrapassagem</t>
   </si>
   <si>
     <t>Consumo HP</t>
@@ -135,16 +126,10 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Demanda Contratada P Atual:</t>
-  </si>
-  <si>
-    <t>Demanda Contratada FP Atual:</t>
-  </si>
-  <si>
-    <t>Demanda Contratada P Recomendada:</t>
-  </si>
-  <si>
-    <t>Demanda Contratada FP Recomendada:</t>
+    <t>Demanda Contratada Atual:</t>
+  </si>
+  <si>
+    <t>Demanda Contratada Recomendada:</t>
   </si>
   <si>
     <t>Custo - Verde</t>
@@ -153,28 +138,37 @@
     <t>Custo - Azul</t>
   </si>
   <si>
-    <t>Utilizada FP</t>
-  </si>
-  <si>
-    <t>Utilizada P</t>
-  </si>
-  <si>
-    <t>Contratada FP - 153 kW</t>
-  </si>
-  <si>
-    <t>Contratada P - 153 kW</t>
-  </si>
-  <si>
-    <t>Proposta FP - 150 kW</t>
-  </si>
-  <si>
-    <t>Proposta P - 145 kW</t>
-  </si>
-  <si>
-    <t>Proposta + Tolerância de 5% (FP)</t>
-  </si>
-  <si>
-    <t>Proposta + Tolerância de 5% (P)</t>
+    <t>Utilizada</t>
+  </si>
+  <si>
+    <t>Contratada - 150 kW</t>
+  </si>
+  <si>
+    <t>Proposta - 105 kW</t>
+  </si>
+  <si>
+    <t>Proposta + Tolerância de 5%</t>
+  </si>
+  <si>
+    <t>Custo</t>
+  </si>
+  <si>
+    <t>Demanda Contratada Atual</t>
+  </si>
+  <si>
+    <t>Demanda Contratada Recomendada</t>
+  </si>
+  <si>
+    <t>Demandas Contratadas</t>
+  </si>
+  <si>
+    <t>Custos Anuais</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
   </si>
 </sst>
 </file>
@@ -369,85 +363,85 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>JAN/23</c:v>
+                  <c:v>MAI/23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEV/23</c:v>
+                  <c:v>JUN/23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR/23</c:v>
+                  <c:v>JUL/23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ABR/23</c:v>
+                  <c:v>AGO/23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>MAI/23</c:v>
+                  <c:v>SET/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>JUN/23</c:v>
+                  <c:v>OUT/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>JUL/23</c:v>
+                  <c:v>NOV/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AGO/23</c:v>
+                  <c:v>DEZ/23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SET/23</c:v>
+                  <c:v>JAN/24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>OUT/23</c:v>
+                  <c:v>FEV/24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>NOV/23</c:v>
+                  <c:v>MAR/24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>DEZ/23</c:v>
+                  <c:v>ABR/24</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$O$2:$O$13</c:f>
+              <c:f>Geral!$L$2:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4315.5976059</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3852.2527284</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3470.7111957</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3839.6391015</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3811.6927425</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4444.1112936</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4348.7160195</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4775.5795689</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4112.646615</c:v>
+                  <c:v>3.48025056</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5998.4216019</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4126.7312922</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3384.9838512</c:v>
+                  <c:v>1.74012528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,7 +460,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$Q$2:$Q$13</c:f>
+              <c:f>Geral!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -534,7 +528,7 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="'R$ #,##0.00'" sourceLinked="0"/>
+        <c:numFmt formatCode="R$ #,##0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -585,40 +579,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>JAN/23</c:v>
+                  <c:v>MAI/23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEV/23</c:v>
+                  <c:v>JUN/23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR/23</c:v>
+                  <c:v>JUL/23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ABR/23</c:v>
+                  <c:v>AGO/23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>MAI/23</c:v>
+                  <c:v>SET/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>JUN/23</c:v>
+                  <c:v>OUT/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>JUL/23</c:v>
+                  <c:v>NOV/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AGO/23</c:v>
+                  <c:v>DEZ/23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SET/23</c:v>
+                  <c:v>JAN/24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>OUT/23</c:v>
+                  <c:v>FEV/24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>NOV/23</c:v>
+                  <c:v>MAR/24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>DEZ/23</c:v>
+                  <c:v>ABR/24</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -630,40 +624,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>53140.07998734999</c:v>
+                  <c:v>14415.18882735104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55086.30186711</c:v>
+                  <c:v>14823.60068641152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49586.23364305</c:v>
+                  <c:v>13230.19634161792</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55506.98194519</c:v>
+                  <c:v>13955.17430689984</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52203.70853644</c:v>
+                  <c:v>17734.35150544704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56061.31273675</c:v>
+                  <c:v>21124.5244156224</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55716.93268549</c:v>
+                  <c:v>21604.04689938304</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57985.01330517</c:v>
+                  <c:v>22465.53536750272</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59765.05869915</c:v>
+                  <c:v>15035.4673131936</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63440.23088899</c:v>
+                  <c:v>11455.2858804544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60509.37502902</c:v>
+                  <c:v>10347.47630204096</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>57678.02190802</c:v>
+                  <c:v>11809.26164385984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -693,40 +687,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>52280.7708684</c:v>
+                  <c:v>15983.68717710104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53284.02397394</c:v>
+                  <c:v>16103.39225836152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49815.18206370001</c:v>
+                  <c:v>14683.07081266792</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53292.08245626</c:v>
+                  <c:v>15309.49854574984</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52482.73257576</c:v>
+                  <c:v>18469.77036619704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53849.5676175</c:v>
+                  <c:v>22198.84626944443</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53419.23099246</c:v>
+                  <c:v>23914.28630773989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56080.0023798</c:v>
+                  <c:v>27012.64845911814</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56160.84712628</c:v>
+                  <c:v>16432.4088998436</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59910.65219158</c:v>
+                  <c:v>12608.8469285044</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57597.84625278</c:v>
+                  <c:v>11663.05307236755</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55329.24538833999</c:v>
+                  <c:v>13749.06787502131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,7 +813,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Demanda Contratada X Demanda Recomendada (FP)</a:t>
+              <a:t>Demanda Contratada X Demanda Recomendada</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -839,7 +833,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Utilizada FP</c:v>
+                  <c:v>Utilizada</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -860,40 +854,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>JAN/23</c:v>
+                  <c:v>MAI/23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEV/23</c:v>
+                  <c:v>JUN/23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR/23</c:v>
+                  <c:v>JUL/23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ABR/23</c:v>
+                  <c:v>AGO/23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>MAI/23</c:v>
+                  <c:v>SET/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>JUN/23</c:v>
+                  <c:v>OUT/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>JUL/23</c:v>
+                  <c:v>NOV/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AGO/23</c:v>
+                  <c:v>DEZ/23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SET/23</c:v>
+                  <c:v>JAN/24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>OUT/23</c:v>
+                  <c:v>FEV/24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>NOV/23</c:v>
+                  <c:v>MAR/24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>DEZ/23</c:v>
+                  <c:v>ABR/24</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -905,40 +899,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>140.28</c:v>
+                  <c:v>108.4368</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>137.76</c:v>
+                  <c:v>87.9696</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142.8</c:v>
+                  <c:v>88.1664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136.08</c:v>
+                  <c:v>80.688</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138.6</c:v>
+                  <c:v>110.208</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>132.72</c:v>
+                  <c:v>137.1696</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137.76</c:v>
+                  <c:v>137.3664</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153.3</c:v>
+                  <c:v>138.3504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>154.98</c:v>
+                  <c:v>106.8624</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>157.5</c:v>
+                  <c:v>75.9648</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>162.96</c:v>
+                  <c:v>95.6448</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>157.08</c:v>
+                  <c:v>96.23520000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,11 +944,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$D$1</c:f>
+              <c:f>'Recomendação'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Contratada FP - 153 kW</c:v>
+                  <c:v>Contratada - 150 kW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -971,45 +965,45 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$D$2:$D$13</c:f>
+              <c:f>'Recomendação'!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>153</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,11 +1014,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$F$1</c:f>
+              <c:f>'Recomendação'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Proposta FP - 150 kW</c:v>
+                  <c:v>Proposta - 105 kW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1041,45 +1035,45 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$F$2:$F$13</c:f>
+              <c:f>'Recomendação'!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>150</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,11 +1084,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$H$1</c:f>
+              <c:f>'Recomendação'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Proposta + Tolerância de 5% (FP)</c:v>
+                  <c:v>Proposta + Tolerância de 5%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1112,45 +1106,45 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$H$2:$H$13</c:f>
+              <c:f>'Recomendação'!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>157.5</c:v>
+                  <c:v>110.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1241,7 +1235,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Demanda Contratada X Demanda Recomendada (P)</a:t>
+              <a:t>Custo Anual X Demanda Contratada</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1257,11 +1251,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$C$1</c:f>
+              <c:f>'Recomendação'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Utilizada P</c:v>
+                  <c:v>Custos Anuais</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1277,90 +1271,313 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'Recomendação'!$A$2:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
+            <c:numRef>
+              <c:f>'Recomendação'!$G$2:$G$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>JAN/23</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEV/23</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR/23</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ABR/23</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>MAI/23</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>JUN/23</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>JUL/23</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AGO/23</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SET/23</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>OUT/23</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>NOV/23</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>DEZ/23</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>245</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$C$2:$C$13</c:f>
+              <c:f>'Recomendação'!$H$2:$H$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>122.22</c:v>
+                  <c:v>117302.2122811392</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129.78</c:v>
+                  <c:v>113465.8679611392</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127.26</c:v>
+                  <c:v>109629.5236411392</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>124.32</c:v>
+                  <c:v>105793.1793211392</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>126</c:v>
+                  <c:v>101956.8350011392</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>123.9</c:v>
+                  <c:v>98120.4906811392</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124.74</c:v>
+                  <c:v>94284.14636113921</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>151.62</c:v>
+                  <c:v>90447.80204113921</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140.7</c:v>
+                  <c:v>86611.4577211392</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>147.42</c:v>
+                  <c:v>82775.1134011392</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>147.42</c:v>
+                  <c:v>78938.76908113919</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>148.68</c:v>
+                  <c:v>75102.42476113921</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71266.0804411392</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>67429.7361211392</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>63531.7033844736</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60100.0678146048</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>56808.4843880448</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>54694.14715514881</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52655.7695397888</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>51636.58073210881</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50005.67403479041</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50155.9564296192</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50628.84980613121</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>51108.3928461312</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>51587.9358861312</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52067.4789261312</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>52042.77286871041</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>53708.82048000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>55626.99264</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>57545.1648</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>59463.33696</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61381.50912</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>63299.68128</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>65217.85344000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>67136.02560000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>69054.19776000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>70972.36992</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>72890.54208</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>74808.71424</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>76726.8864</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>78645.05856</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>80563.23072000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>82481.40288000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>84399.57504</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>86317.74720000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>88235.91936</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>90154.09152</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>92072.26368</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>93990.43584000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,66 +1589,37 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$E$1</c:f>
+              <c:f>'Recomendação'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Contratada P - 153 kW</c:v>
+                  <c:v>Column3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="C0504D"/>
-              </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="R$ #,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$E$2:$E$13</c:f>
+              <c:f>'Recomendação'!$I$2:$I$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>153</c:v>
+                <c:ptCount val="49"/>
+                <c:pt idx="29">
+                  <c:v>57545.1648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1442,137 +1630,37 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$G$1</c:f>
+              <c:f>'Recomendação'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Proposta P - 145 kW</c:v>
+                  <c:v>Column4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="R$ #,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$G$2:$G$13</c:f>
+              <c:f>'Recomendação'!$J$2:$J$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>145</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Recomendação'!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Proposta + Tolerância de 5% (P)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="lgDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Recomendação'!$I$2:$I$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>152.25</c:v>
+                <c:ptCount val="49"/>
+                <c:pt idx="20">
+                  <c:v>50005.67403479041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,7 +1676,36 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Demandas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="50040002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1613,7 +1730,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Demanda - kW</a:t>
+                  <a:t>Custos Anuais</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1658,8 +1775,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -1754,13 +1871,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1784,44 +1901,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q13" totalsRowShown="0">
-  <autoFilter ref="A1:Q13"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N13" totalsRowShown="0">
+  <autoFilter ref="A1:N13"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="Mês"/>
     <tableColumn id="2" name="Demanda Registrada HP"/>
-    <tableColumn id="3" name="Custo Demanda HP"/>
-    <tableColumn id="4" name="Demanda Registrada HFP"/>
-    <tableColumn id="5" name="Custo Demanda HFP"/>
-    <tableColumn id="6" name="Ultrapassagem Registrada HP"/>
-    <tableColumn id="7" name="Custo Ultrapassagem HP"/>
-    <tableColumn id="8" name="Ultrapassagem Registrada HFP"/>
-    <tableColumn id="9" name="Custo Ultrapassagem HFP"/>
-    <tableColumn id="10" name="Consumo HP"/>
-    <tableColumn id="11" name="Custo Consumo HP"/>
-    <tableColumn id="12" name="Consumo HFP"/>
-    <tableColumn id="13" name="Custo Consumo HFP"/>
-    <tableColumn id="14" name="Energia Reativa"/>
-    <tableColumn id="15" name="Custo Energia Reativa"/>
-    <tableColumn id="16" name="Demanda Reativa"/>
-    <tableColumn id="17" name="Custo Demanda Reativa"/>
+    <tableColumn id="3" name="Demanda Registrada HFP"/>
+    <tableColumn id="4" name="Custo Demanda"/>
+    <tableColumn id="5" name="Ultrapassagem Registrada"/>
+    <tableColumn id="6" name="Custo Ultrapassagem"/>
+    <tableColumn id="7" name="Consumo HP"/>
+    <tableColumn id="8" name="Custo Consumo HP"/>
+    <tableColumn id="9" name="Consumo HFP"/>
+    <tableColumn id="10" name="Custo Consumo HFP"/>
+    <tableColumn id="11" name="Energia Reativa"/>
+    <tableColumn id="12" name="Custo Energia Reativa"/>
+    <tableColumn id="13" name="Demanda Reativa"/>
+    <tableColumn id="14" name="Custo Demanda Reativa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I13" totalsRowShown="0">
-  <autoFilter ref="A1:I13"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Mês"/>
-    <tableColumn id="2" name="Utilizada FP"/>
-    <tableColumn id="3" name="Utilizada P"/>
-    <tableColumn id="4" name="Contratada FP - 153 kW"/>
-    <tableColumn id="5" name="Contratada P - 153 kW"/>
-    <tableColumn id="6" name="Proposta FP - 150 kW"/>
-    <tableColumn id="7" name="Proposta P - 145 kW"/>
-    <tableColumn id="8" name="Proposta + Tolerância de 5% (FP)"/>
-    <tableColumn id="9" name="Proposta + Tolerância de 5% (P)"/>
+    <tableColumn id="2" name="Utilizada"/>
+    <tableColumn id="3" name="Contratada - 150 kW"/>
+    <tableColumn id="4" name="Proposta - 105 kW"/>
+    <tableColumn id="5" name="Proposta + Tolerância de 5%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="G1:J50" totalsRowShown="0">
+  <autoFilter ref="G1:J50"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Demandas Contratadas"/>
+    <tableColumn id="2" name="Custos Anuais"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2112,7 +2235,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2120,24 +2243,21 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2180,649 +2300,532 @@
       <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>122.22</v>
+        <v>37.5888</v>
       </c>
       <c r="C2">
-        <v>9474.037419419999</v>
+        <v>108.4368</v>
       </c>
       <c r="D2">
-        <v>140.28</v>
+        <v>4795.4304</v>
       </c>
       <c r="E2">
-        <v>4506.84962784</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1035.61</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>2671.0867364</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>17825.16</v>
       </c>
       <c r="J2">
-        <v>6443.95</v>
+        <v>8277.42790962624</v>
       </c>
       <c r="K2">
-        <v>4259.3349589</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>68491.5</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>31962.4488645</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>11998.77</v>
-      </c>
-      <c r="O2">
-        <v>4315.5976059</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>129.78</v>
+        <v>34.8336</v>
       </c>
       <c r="C3">
-        <v>10060.06035258</v>
+        <v>87.9696</v>
       </c>
       <c r="D3">
-        <v>137.76</v>
+        <v>4795.4304</v>
       </c>
       <c r="E3">
-        <v>4425.888257279999</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1186.95</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>3061.428918</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>18100.68</v>
       </c>
       <c r="J3">
-        <v>6946.17</v>
+        <v>8405.37048841152</v>
       </c>
       <c r="K3">
-        <v>4591.29333894</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>69930</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>32633.74359</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>10710.52</v>
-      </c>
-      <c r="O3">
-        <v>3852.2527284</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>127.26</v>
+        <v>40.1472</v>
       </c>
       <c r="C4">
-        <v>9864.71937486</v>
+        <v>88.1664</v>
       </c>
       <c r="D4">
-        <v>142.8</v>
+        <v>4795.4304</v>
       </c>
       <c r="E4">
-        <v>4587.8109984</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1096.22</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>2827.4144728</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>15173.28</v>
       </c>
       <c r="J4">
-        <v>5864.35</v>
+        <v>7045.980588817921</v>
       </c>
       <c r="K4">
-        <v>3876.2297917</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>64029</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>29879.965227</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>9649.709999999999</v>
-      </c>
-      <c r="O4">
-        <v>3470.7111957</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>124.32</v>
+        <v>33.6528</v>
       </c>
       <c r="C5">
-        <v>9636.821567519999</v>
+        <v>80.688</v>
       </c>
       <c r="D5">
-        <v>136.08</v>
+        <v>4795.4304</v>
       </c>
       <c r="E5">
-        <v>4371.91401024</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1147.88</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>2960.6580112</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>16447.56</v>
       </c>
       <c r="J5">
-        <v>7165.93</v>
+        <v>7637.71501569984</v>
       </c>
       <c r="K5">
-        <v>4736.55074326</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>69636</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>32496.544668</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>10675.45</v>
-      </c>
-      <c r="O5">
-        <v>3839.6391015</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>126</v>
+        <v>44.4768</v>
       </c>
       <c r="C6">
-        <v>9767.048886</v>
+        <v>110.208</v>
       </c>
       <c r="D6">
-        <v>138.6</v>
+        <v>4795.4304</v>
       </c>
       <c r="E6">
-        <v>4452.875380799999</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1472.31</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>3797.4408444</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>22425.36</v>
       </c>
       <c r="J6">
-        <v>5837.68</v>
+        <v>10413.61203755904</v>
       </c>
       <c r="K6">
-        <v>3858.60140176</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>69783</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>32565.144129</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>10597.75</v>
-      </c>
-      <c r="O6">
-        <v>3811.6927425</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>123.9</v>
+        <v>47.0352</v>
       </c>
       <c r="C7">
-        <v>9604.264737900001</v>
+        <v>137.1696</v>
       </c>
       <c r="D7">
-        <v>132.72</v>
+        <v>4795.4304</v>
       </c>
       <c r="E7">
-        <v>4263.965516159999</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1378.68</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>3555.9466032</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>23960.4</v>
       </c>
       <c r="J7">
-        <v>7164.25</v>
+        <v>11126.4349765056</v>
       </c>
       <c r="K7">
-        <v>4735.4402935</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>70833</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>33055.140279</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>12356.08</v>
-      </c>
-      <c r="O7">
-        <v>4444.1112936</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>124.74</v>
+        <v>50.5776</v>
       </c>
       <c r="C8">
-        <v>9669.378397139999</v>
+        <v>137.3664</v>
       </c>
       <c r="D8">
-        <v>137.76</v>
+        <v>4795.4304</v>
       </c>
       <c r="E8">
-        <v>4425.888257279999</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1337.6</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>3449.991424</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>25180.56</v>
       </c>
       <c r="J8">
-        <v>7210.03</v>
+        <v>11693.03782541184</v>
       </c>
       <c r="K8">
-        <v>4765.70004946</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>69846</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>32594.543898</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>12090.85</v>
-      </c>
-      <c r="O8">
-        <v>4348.7160195</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>151.62</v>
+        <v>62.1888</v>
       </c>
       <c r="C9">
-        <v>11753.01549282</v>
+        <v>138.3504</v>
       </c>
       <c r="D9">
-        <v>153.3</v>
+        <v>4795.4304</v>
       </c>
       <c r="E9">
-        <v>4925.1500424</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1603.13</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>4134.8570212</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>25357.68</v>
       </c>
       <c r="J9">
-        <v>7274.19</v>
+        <v>11775.28662605952</v>
       </c>
       <c r="K9">
-        <v>4808.108654579999</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>74130</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>34593.72819</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>13277.67</v>
-      </c>
-      <c r="O9">
-        <v>4775.5795689</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>140.7</v>
+        <v>40.344</v>
       </c>
       <c r="C10">
-        <v>10906.5379227</v>
+        <v>106.8624</v>
       </c>
       <c r="D10">
-        <v>154.98</v>
+        <v>4795.4304</v>
       </c>
       <c r="E10">
-        <v>4979.124289439999</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1125.54</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>2903.0377896</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>18769.8</v>
       </c>
       <c r="J10">
-        <v>7905.87</v>
+        <v>8716.088179747201</v>
       </c>
       <c r="K10">
-        <v>5225.637764339999</v>
+        <v>9.84</v>
       </c>
       <c r="L10">
-        <v>74392.5</v>
+        <v>3.48025056</v>
       </c>
       <c r="M10">
-        <v>34716.2272275</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>11434.5</v>
-      </c>
-      <c r="O10">
-        <v>4112.646615</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>147.42</v>
+        <v>39.7536</v>
       </c>
       <c r="C11">
-        <v>11427.44719662</v>
+        <v>75.9648</v>
       </c>
       <c r="D11">
-        <v>157.5</v>
+        <v>4795.4304</v>
       </c>
       <c r="E11">
-        <v>5060.08566</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1253.12</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>3232.0972288</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>10479.6</v>
       </c>
       <c r="J11">
-        <v>7966.03</v>
+        <v>4866.3873716544</v>
       </c>
       <c r="K11">
-        <v>5265.40244146</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>80734.5</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>37675.8039735</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>16677.57</v>
-      </c>
-      <c r="O11">
-        <v>5998.4216019</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>147.42</v>
+        <v>46.0512</v>
       </c>
       <c r="C12">
-        <v>11427.44719662</v>
+        <v>95.6448</v>
       </c>
       <c r="D12">
-        <v>162.96</v>
+        <v>4795.4304</v>
       </c>
       <c r="E12">
-        <v>5235.50196288</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1211.59</v>
       </c>
       <c r="H12">
-        <v>9.960000000000008</v>
+        <v>3124.9813916</v>
       </c>
       <c r="I12">
-        <v>639.9803577600005</v>
+        <v>8324.639999999999</v>
       </c>
       <c r="J12">
-        <v>7636.86</v>
+        <v>3865.69363044096</v>
       </c>
       <c r="K12">
-        <v>5047.82699652</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>75117</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>35054.324571</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>11473.66</v>
-      </c>
-      <c r="O12">
-        <v>4126.7312922</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>148.68</v>
+        <v>48.8064</v>
       </c>
       <c r="C13">
-        <v>11525.11768548</v>
+        <v>96.23520000000001</v>
       </c>
       <c r="D13">
-        <v>157.08</v>
+        <v>4795.4304</v>
       </c>
       <c r="E13">
-        <v>5046.59209824</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1312.41</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>3385.0203684</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>10912.56</v>
       </c>
       <c r="J13">
-        <v>7389.16</v>
+        <v>5067.43999545984</v>
       </c>
       <c r="K13">
-        <v>4884.101755119999</v>
+        <v>4.92</v>
       </c>
       <c r="L13">
-        <v>72586.5</v>
+        <v>1.74012528</v>
       </c>
       <c r="M13">
-        <v>33873.4338495</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>9411.360000000001</v>
-      </c>
-      <c r="O13">
-        <v>3384.9838512</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
         <v>0</v>
       </c>
     </row>
@@ -2837,7 +2840,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2849,48 +2852,48 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -2900,11 +2903,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2918,11 +2921,11 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -2930,71 +2933,71 @@
     <row r="3" spans="1:25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -3002,10 +3005,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="3">
-        <v>140.28</v>
+        <v>108.4368</v>
       </c>
       <c r="C4" s="4">
-        <v>4819.129199999999</v>
+        <v>3466.6741813248</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -3014,28 +3017,28 @@
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <v>6443.95</v>
+        <v>1035.61</v>
       </c>
       <c r="G4" s="4">
-        <v>16358.50192285</v>
+        <v>2671.0867364</v>
       </c>
       <c r="H4" s="5">
-        <v>68491.5</v>
+        <v>17825.16</v>
       </c>
       <c r="I4" s="4">
-        <v>31962.4488645</v>
+        <v>8277.42790962624</v>
       </c>
       <c r="J4" s="4">
-        <v>53140.07998734999</v>
+        <v>14415.18882735104</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="M4" s="6">
-        <v>122.22</v>
+        <v>37.5888</v>
       </c>
       <c r="N4" s="7">
-        <v>11239.857845</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O4" s="6">
         <v>0</v>
@@ -3044,10 +3047,10 @@
         <v>0</v>
       </c>
       <c r="Q4" s="6">
-        <v>140.28</v>
+        <v>108.4368</v>
       </c>
       <c r="R4" s="7">
-        <v>4819.129199999999</v>
+        <v>3466.6741813248</v>
       </c>
       <c r="S4" s="6">
         <v>0</v>
@@ -3056,19 +3059,19 @@
         <v>0</v>
       </c>
       <c r="U4" s="8">
-        <v>6443.95</v>
+        <v>1035.61</v>
       </c>
       <c r="V4" s="7">
-        <v>4259.3349589</v>
+        <v>695.4846077</v>
       </c>
       <c r="W4" s="8">
-        <v>68491.5</v>
+        <v>17825.16</v>
       </c>
       <c r="X4" s="7">
-        <v>31962.4488645</v>
+        <v>8277.42790962624</v>
       </c>
       <c r="Y4" s="7">
-        <v>52280.7708684</v>
+        <v>15983.68717710104</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -3076,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>137.76</v>
+        <v>87.9696</v>
       </c>
       <c r="C5" s="4">
-        <v>4819.129199999999</v>
+        <v>3356.80128</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -3088,28 +3091,28 @@
         <v>0</v>
       </c>
       <c r="F5" s="5">
-        <v>6946.17</v>
+        <v>1186.95</v>
       </c>
       <c r="G5" s="4">
-        <v>17633.42907711</v>
+        <v>3061.428918</v>
       </c>
       <c r="H5" s="5">
-        <v>69930</v>
+        <v>18100.68</v>
       </c>
       <c r="I5" s="4">
-        <v>32633.74359</v>
+        <v>8405.37048841152</v>
       </c>
       <c r="J5" s="4">
-        <v>55086.30186711</v>
+        <v>14823.60068641152</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M5" s="6">
-        <v>129.78</v>
+        <v>34.8336</v>
       </c>
       <c r="N5" s="7">
-        <v>11239.857845</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O5" s="6">
         <v>0</v>
@@ -3118,10 +3121,10 @@
         <v>0</v>
       </c>
       <c r="Q5" s="6">
-        <v>137.76</v>
+        <v>87.9696</v>
       </c>
       <c r="R5" s="7">
-        <v>4819.129199999999</v>
+        <v>3356.80128</v>
       </c>
       <c r="S5" s="6">
         <v>0</v>
@@ -3130,19 +3133,19 @@
         <v>0</v>
       </c>
       <c r="U5" s="8">
-        <v>6946.17</v>
+        <v>1186.95</v>
       </c>
       <c r="V5" s="7">
-        <v>4591.29333894</v>
+        <v>797.1200115</v>
       </c>
       <c r="W5" s="8">
-        <v>69930</v>
+        <v>18100.68</v>
       </c>
       <c r="X5" s="7">
-        <v>32633.74359</v>
+        <v>8405.37048841152</v>
       </c>
       <c r="Y5" s="7">
-        <v>53284.02397394</v>
+        <v>16103.39225836152</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -3150,10 +3153,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>142.8</v>
+        <v>88.1664</v>
       </c>
       <c r="C6" s="4">
-        <v>4819.129199999999</v>
+        <v>3356.80128</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -3162,28 +3165,28 @@
         <v>0</v>
       </c>
       <c r="F6" s="5">
-        <v>5864.35</v>
+        <v>1096.22</v>
       </c>
       <c r="G6" s="4">
-        <v>14887.13921605</v>
+        <v>2827.4144728</v>
       </c>
       <c r="H6" s="5">
-        <v>64029</v>
+        <v>15173.28</v>
       </c>
       <c r="I6" s="4">
-        <v>29879.965227</v>
+        <v>7045.980588817921</v>
       </c>
       <c r="J6" s="4">
-        <v>49586.23364305</v>
+        <v>13230.19634161792</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M6" s="6">
-        <v>127.26</v>
+        <v>40.1472</v>
       </c>
       <c r="N6" s="7">
-        <v>11239.857845</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O6" s="6">
         <v>0</v>
@@ -3192,10 +3195,10 @@
         <v>0</v>
       </c>
       <c r="Q6" s="6">
-        <v>142.8</v>
+        <v>88.1664</v>
       </c>
       <c r="R6" s="7">
-        <v>4819.129199999999</v>
+        <v>3356.80128</v>
       </c>
       <c r="S6" s="6">
         <v>0</v>
@@ -3204,19 +3207,19 @@
         <v>0</v>
       </c>
       <c r="U6" s="8">
-        <v>5864.35</v>
+        <v>1096.22</v>
       </c>
       <c r="V6" s="7">
-        <v>3876.2297917</v>
+        <v>736.1884654</v>
       </c>
       <c r="W6" s="8">
-        <v>64029</v>
+        <v>15173.28</v>
       </c>
       <c r="X6" s="7">
-        <v>29879.965227</v>
+        <v>7045.980588817921</v>
       </c>
       <c r="Y6" s="7">
-        <v>49815.18206370001</v>
+        <v>14683.07081266792</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -3224,10 +3227,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>136.08</v>
+        <v>80.688</v>
       </c>
       <c r="C7" s="4">
-        <v>4819.129199999999</v>
+        <v>3356.80128</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -3236,28 +3239,28 @@
         <v>0</v>
       </c>
       <c r="F7" s="5">
-        <v>7165.93</v>
+        <v>1147.88</v>
       </c>
       <c r="G7" s="4">
-        <v>18191.30807719</v>
+        <v>2960.6580112</v>
       </c>
       <c r="H7" s="5">
-        <v>69636</v>
+        <v>16447.56</v>
       </c>
       <c r="I7" s="4">
-        <v>32496.544668</v>
+        <v>7637.71501569984</v>
       </c>
       <c r="J7" s="4">
-        <v>55506.98194519</v>
+        <v>13955.17430689984</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M7" s="6">
-        <v>124.32</v>
+        <v>33.6528</v>
       </c>
       <c r="N7" s="7">
-        <v>11239.857845</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O7" s="6">
         <v>0</v>
@@ -3266,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="Q7" s="6">
-        <v>136.08</v>
+        <v>80.688</v>
       </c>
       <c r="R7" s="7">
-        <v>4819.129199999999</v>
+        <v>3356.80128</v>
       </c>
       <c r="S7" s="6">
         <v>0</v>
@@ -3278,19 +3281,19 @@
         <v>0</v>
       </c>
       <c r="U7" s="8">
-        <v>7165.93</v>
+        <v>1147.88</v>
       </c>
       <c r="V7" s="7">
-        <v>4736.55074326</v>
+        <v>770.8817716000001</v>
       </c>
       <c r="W7" s="8">
-        <v>69636</v>
+        <v>16447.56</v>
       </c>
       <c r="X7" s="7">
-        <v>32496.544668</v>
+        <v>7637.71501569984</v>
       </c>
       <c r="Y7" s="7">
-        <v>53292.08245626</v>
+        <v>15309.49854574984</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -3298,10 +3301,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>138.6</v>
+        <v>110.208</v>
       </c>
       <c r="C8" s="4">
-        <v>4819.129199999999</v>
+        <v>3523.298623488</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -3310,28 +3313,28 @@
         <v>0</v>
       </c>
       <c r="F8" s="5">
-        <v>5837.68</v>
+        <v>1472.31</v>
       </c>
       <c r="G8" s="4">
-        <v>14819.43520744</v>
+        <v>3797.4408444</v>
       </c>
       <c r="H8" s="5">
-        <v>69783</v>
+        <v>22425.36</v>
       </c>
       <c r="I8" s="4">
-        <v>32565.144129</v>
+        <v>10413.61203755904</v>
       </c>
       <c r="J8" s="4">
-        <v>52203.70853644</v>
+        <v>17734.35150544704</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M8" s="6">
-        <v>126</v>
+        <v>44.4768</v>
       </c>
       <c r="N8" s="7">
-        <v>11239.857845</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O8" s="6">
         <v>0</v>
@@ -3340,10 +3343,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="6">
-        <v>138.6</v>
+        <v>110.208</v>
       </c>
       <c r="R8" s="7">
-        <v>4819.129199999999</v>
+        <v>3523.298623488</v>
       </c>
       <c r="S8" s="6">
         <v>0</v>
@@ -3352,19 +3355,19 @@
         <v>0</v>
       </c>
       <c r="U8" s="8">
-        <v>5837.68</v>
+        <v>1472.31</v>
       </c>
       <c r="V8" s="7">
-        <v>3858.60140176</v>
+        <v>988.7592267</v>
       </c>
       <c r="W8" s="8">
-        <v>69783</v>
+        <v>22425.36</v>
       </c>
       <c r="X8" s="7">
-        <v>32565.144129</v>
+        <v>10413.61203755904</v>
       </c>
       <c r="Y8" s="7">
-        <v>52482.73257576</v>
+        <v>18469.77036619704</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -3372,40 +3375,40 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>132.72</v>
+        <v>137.1696</v>
       </c>
       <c r="C9" s="4">
-        <v>4819.129199999999</v>
+        <v>4385.2484653056</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>32.1696</v>
       </c>
       <c r="E9" s="4">
-        <v>0</v>
+        <v>2056.8943706112</v>
       </c>
       <c r="F9" s="5">
-        <v>7164.25</v>
+        <v>1378.68</v>
       </c>
       <c r="G9" s="4">
-        <v>18187.04325775</v>
+        <v>3555.9466032</v>
       </c>
       <c r="H9" s="5">
-        <v>70833</v>
+        <v>23960.4</v>
       </c>
       <c r="I9" s="4">
-        <v>33055.140279</v>
+        <v>11126.4349765056</v>
       </c>
       <c r="J9" s="4">
-        <v>56061.31273675</v>
+        <v>21124.5244156224</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M9" s="6">
-        <v>123.9</v>
+        <v>47.0352</v>
       </c>
       <c r="N9" s="7">
-        <v>11239.857845</v>
+        <v>3704.388329422032</v>
       </c>
       <c r="O9" s="6">
         <v>0</v>
@@ -3414,31 +3417,31 @@
         <v>0</v>
       </c>
       <c r="Q9" s="6">
-        <v>132.72</v>
+        <v>137.1696</v>
       </c>
       <c r="R9" s="7">
-        <v>4819.129199999999</v>
+        <v>4385.2484653056</v>
       </c>
       <c r="S9" s="6">
-        <v>0</v>
+        <v>32.1696</v>
       </c>
       <c r="T9" s="7">
-        <v>0</v>
+        <v>2056.8943706112</v>
       </c>
       <c r="U9" s="8">
-        <v>7164.25</v>
+        <v>1378.68</v>
       </c>
       <c r="V9" s="7">
-        <v>4735.4402935</v>
+        <v>925.8801276</v>
       </c>
       <c r="W9" s="8">
-        <v>70833</v>
+        <v>23960.4</v>
       </c>
       <c r="X9" s="7">
-        <v>33055.140279</v>
+        <v>11126.4349765056</v>
       </c>
       <c r="Y9" s="7">
-        <v>53849.5676175</v>
+        <v>22198.84626944443</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -3446,73 +3449,73 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>137.76</v>
+        <v>137.3664</v>
       </c>
       <c r="C10" s="4">
-        <v>4819.129199999999</v>
+        <v>4391.5400699904</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>32.3664</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>2069.4775799808</v>
       </c>
       <c r="F10" s="5">
-        <v>7210.03</v>
+        <v>1337.6</v>
       </c>
       <c r="G10" s="4">
-        <v>18303.25958749</v>
+        <v>3449.991424</v>
       </c>
       <c r="H10" s="5">
-        <v>69846</v>
+        <v>25180.56</v>
       </c>
       <c r="I10" s="4">
-        <v>32594.543898</v>
+        <v>11693.03782541184</v>
       </c>
       <c r="J10" s="4">
-        <v>55716.93268549</v>
+        <v>21604.04689938304</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M10" s="6">
-        <v>124.74</v>
+        <v>50.5776</v>
       </c>
       <c r="N10" s="7">
-        <v>11239.857845</v>
+        <v>3983.379919085616</v>
       </c>
       <c r="O10" s="6">
-        <v>0</v>
+        <v>5.577599999999997</v>
       </c>
       <c r="P10" s="7">
-        <v>0</v>
+        <v>878.5588812712315</v>
       </c>
       <c r="Q10" s="6">
-        <v>137.76</v>
+        <v>137.3664</v>
       </c>
       <c r="R10" s="7">
-        <v>4819.129199999999</v>
+        <v>4391.5400699904</v>
       </c>
       <c r="S10" s="6">
-        <v>0</v>
+        <v>32.3664</v>
       </c>
       <c r="T10" s="7">
-        <v>0</v>
+        <v>2069.4775799808</v>
       </c>
       <c r="U10" s="8">
-        <v>7210.03</v>
+        <v>1337.6</v>
       </c>
       <c r="V10" s="7">
-        <v>4765.70004946</v>
+        <v>898.2920319999999</v>
       </c>
       <c r="W10" s="8">
-        <v>69846</v>
+        <v>25180.56</v>
       </c>
       <c r="X10" s="7">
-        <v>32594.543898</v>
+        <v>11693.03782541184</v>
       </c>
       <c r="Y10" s="7">
-        <v>53419.23099246</v>
+        <v>23914.28630773989</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -3520,73 +3523,73 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>153.3</v>
+        <v>138.3504</v>
       </c>
       <c r="C11" s="4">
-        <v>4925.1500424</v>
+        <v>4422.998093414401</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>33.35040000000001</v>
       </c>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>2132.393626828801</v>
       </c>
       <c r="F11" s="5">
-        <v>7274.19</v>
+        <v>1603.13</v>
       </c>
       <c r="G11" s="4">
-        <v>18466.13507277</v>
+        <v>4134.8570212</v>
       </c>
       <c r="H11" s="5">
-        <v>74130</v>
+        <v>25357.68</v>
       </c>
       <c r="I11" s="4">
-        <v>34593.72819</v>
+        <v>11775.28662605952</v>
       </c>
       <c r="J11" s="4">
-        <v>57985.01330517</v>
+        <v>22465.53536750272</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M11" s="6">
-        <v>151.62</v>
+        <v>62.1888</v>
       </c>
       <c r="N11" s="7">
-        <v>11753.01549282</v>
+        <v>4897.852351871808</v>
       </c>
       <c r="O11" s="6">
-        <v>0</v>
+        <v>17.1888</v>
       </c>
       <c r="P11" s="7">
-        <v>0</v>
+        <v>2707.503746843616</v>
       </c>
       <c r="Q11" s="6">
-        <v>153.3</v>
+        <v>138.3504</v>
       </c>
       <c r="R11" s="7">
-        <v>4925.1500424</v>
+        <v>4422.998093414401</v>
       </c>
       <c r="S11" s="6">
-        <v>0</v>
+        <v>33.35040000000001</v>
       </c>
       <c r="T11" s="7">
-        <v>0</v>
+        <v>2132.393626828801</v>
       </c>
       <c r="U11" s="8">
-        <v>7274.19</v>
+        <v>1603.13</v>
       </c>
       <c r="V11" s="7">
-        <v>4808.108654579999</v>
+        <v>1076.6140141</v>
       </c>
       <c r="W11" s="8">
-        <v>74130</v>
+        <v>25357.68</v>
       </c>
       <c r="X11" s="7">
-        <v>34593.72819</v>
+        <v>11775.28662605952</v>
       </c>
       <c r="Y11" s="7">
-        <v>56080.0023798</v>
+        <v>27012.64845911814</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -3594,10 +3597,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>154.98</v>
+        <v>106.8624</v>
       </c>
       <c r="C12" s="4">
-        <v>4979.124289439999</v>
+        <v>3416.3413438464</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -3606,28 +3609,28 @@
         <v>0</v>
       </c>
       <c r="F12" s="5">
-        <v>7905.87</v>
+        <v>1125.54</v>
       </c>
       <c r="G12" s="4">
-        <v>20069.70718221</v>
+        <v>2903.0377896</v>
       </c>
       <c r="H12" s="5">
-        <v>74392.5</v>
+        <v>18769.8</v>
       </c>
       <c r="I12" s="4">
-        <v>34716.2272275</v>
+        <v>8716.088179747201</v>
       </c>
       <c r="J12" s="4">
-        <v>59765.05869915</v>
+        <v>15035.4673131936</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="6">
-        <v>140.7</v>
+        <v>40.344</v>
       </c>
       <c r="N12" s="7">
-        <v>11239.857845</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O12" s="6">
         <v>0</v>
@@ -3636,10 +3639,10 @@
         <v>0</v>
       </c>
       <c r="Q12" s="6">
-        <v>154.98</v>
+        <v>106.8624</v>
       </c>
       <c r="R12" s="7">
-        <v>4979.124289439999</v>
+        <v>3416.3413438464</v>
       </c>
       <c r="S12" s="6">
         <v>0</v>
@@ -3648,19 +3651,19 @@
         <v>0</v>
       </c>
       <c r="U12" s="8">
-        <v>7905.87</v>
+        <v>1125.54</v>
       </c>
       <c r="V12" s="7">
-        <v>5225.637764339999</v>
+        <v>755.8788978</v>
       </c>
       <c r="W12" s="8">
-        <v>74392.5</v>
+        <v>18769.8</v>
       </c>
       <c r="X12" s="7">
-        <v>34716.2272275</v>
+        <v>8716.088179747201</v>
       </c>
       <c r="Y12" s="7">
-        <v>56160.84712628</v>
+        <v>16432.4088998436</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -3668,40 +3671,40 @@
         <v>9</v>
       </c>
       <c r="B13" s="3">
-        <v>157.5</v>
+        <v>75.9648</v>
       </c>
       <c r="C13" s="4">
-        <v>5060.08566</v>
+        <v>3356.80128</v>
       </c>
       <c r="D13" s="3">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="E13" s="4">
-        <v>481.91292</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5">
-        <v>7966.03</v>
+        <v>1253.12</v>
       </c>
       <c r="G13" s="4">
-        <v>20222.42833549</v>
+        <v>3232.0972288</v>
       </c>
       <c r="H13" s="5">
-        <v>80734.5</v>
+        <v>10479.6</v>
       </c>
       <c r="I13" s="4">
-        <v>37675.8039735</v>
+        <v>4866.3873716544</v>
       </c>
       <c r="J13" s="4">
-        <v>63440.23088899</v>
+        <v>11455.2858804544</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M13" s="6">
-        <v>147.42</v>
+        <v>39.7536</v>
       </c>
       <c r="N13" s="7">
-        <v>11427.44719662</v>
+        <v>3544.10047845</v>
       </c>
       <c r="O13" s="6">
         <v>0</v>
@@ -3710,31 +3713,31 @@
         <v>0</v>
       </c>
       <c r="Q13" s="6">
-        <v>157.5</v>
+        <v>75.9648</v>
       </c>
       <c r="R13" s="7">
-        <v>5060.08566</v>
+        <v>3356.80128</v>
       </c>
       <c r="S13" s="6">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="T13" s="7">
-        <v>481.91292</v>
+        <v>0</v>
       </c>
       <c r="U13" s="8">
-        <v>7966.03</v>
+        <v>1253.12</v>
       </c>
       <c r="V13" s="7">
-        <v>5265.40244146</v>
+        <v>841.5577983999999</v>
       </c>
       <c r="W13" s="8">
-        <v>80734.5</v>
+        <v>10479.6</v>
       </c>
       <c r="X13" s="7">
-        <v>37675.8039735</v>
+        <v>4866.3873716544</v>
       </c>
       <c r="Y13" s="7">
-        <v>59910.65219158</v>
+        <v>12608.8469285044</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -3742,40 +3745,40 @@
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>162.96</v>
+        <v>95.6448</v>
       </c>
       <c r="C14" s="4">
-        <v>5235.50196288</v>
+        <v>3356.80128</v>
       </c>
       <c r="D14" s="3">
-        <v>12.96000000000001</v>
+        <v>0</v>
       </c>
       <c r="E14" s="4">
-        <v>832.7455257600004</v>
+        <v>0</v>
       </c>
       <c r="F14" s="5">
-        <v>7636.86</v>
+        <v>1211.59</v>
       </c>
       <c r="G14" s="4">
-        <v>19386.80296938</v>
+        <v>3124.9813916</v>
       </c>
       <c r="H14" s="5">
-        <v>75117</v>
+        <v>8324.639999999999</v>
       </c>
       <c r="I14" s="4">
-        <v>35054.324571</v>
+        <v>3865.69363044096</v>
       </c>
       <c r="J14" s="4">
-        <v>60509.37502902</v>
+        <v>10347.47630204096</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M14" s="6">
-        <v>147.42</v>
+        <v>46.0512</v>
       </c>
       <c r="N14" s="7">
-        <v>11427.44719662</v>
+        <v>3626.890665626592</v>
       </c>
       <c r="O14" s="6">
         <v>0</v>
@@ -3784,31 +3787,31 @@
         <v>0</v>
       </c>
       <c r="Q14" s="6">
-        <v>162.96</v>
+        <v>95.6448</v>
       </c>
       <c r="R14" s="7">
-        <v>5235.50196288</v>
+        <v>3356.80128</v>
       </c>
       <c r="S14" s="6">
-        <v>12.96000000000001</v>
+        <v>0</v>
       </c>
       <c r="T14" s="7">
-        <v>832.7455257600004</v>
+        <v>0</v>
       </c>
       <c r="U14" s="8">
-        <v>7636.86</v>
+        <v>1211.59</v>
       </c>
       <c r="V14" s="7">
-        <v>5047.82699652</v>
+        <v>813.6674962999999</v>
       </c>
       <c r="W14" s="8">
-        <v>75117</v>
+        <v>8324.639999999999</v>
       </c>
       <c r="X14" s="7">
-        <v>35054.324571</v>
+        <v>3865.69363044096</v>
       </c>
       <c r="Y14" s="7">
-        <v>57597.84625278</v>
+        <v>11663.05307236755</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -3816,10 +3819,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="3">
-        <v>157.08</v>
+        <v>96.23520000000001</v>
       </c>
       <c r="C15" s="4">
-        <v>5046.59209824</v>
+        <v>3356.80128</v>
       </c>
       <c r="D15" s="3">
         <v>0</v>
@@ -3828,40 +3831,40 @@
         <v>0</v>
       </c>
       <c r="F15" s="5">
-        <v>7389.16</v>
+        <v>1312.41</v>
       </c>
       <c r="G15" s="4">
-        <v>18757.99596028</v>
+        <v>3385.0203684</v>
       </c>
       <c r="H15" s="5">
-        <v>72586.5</v>
+        <v>10912.56</v>
       </c>
       <c r="I15" s="4">
-        <v>33873.4338495</v>
+        <v>5067.43999545984</v>
       </c>
       <c r="J15" s="4">
-        <v>57678.02190802</v>
+        <v>11809.26164385984</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M15" s="6">
-        <v>148.68</v>
+        <v>48.8064</v>
       </c>
       <c r="N15" s="7">
-        <v>11525.11768548</v>
+        <v>3843.884124253824</v>
       </c>
       <c r="O15" s="6">
-        <v>0</v>
+        <v>3.806399999999996</v>
       </c>
       <c r="P15" s="7">
-        <v>0</v>
+        <v>599.5672916076475</v>
       </c>
       <c r="Q15" s="6">
-        <v>157.08</v>
+        <v>96.23520000000001</v>
       </c>
       <c r="R15" s="7">
-        <v>5046.59209824</v>
+        <v>3356.80128</v>
       </c>
       <c r="S15" s="6">
         <v>0</v>
@@ -3870,63 +3873,49 @@
         <v>0</v>
       </c>
       <c r="U15" s="8">
-        <v>7389.16</v>
+        <v>1312.41</v>
       </c>
       <c r="V15" s="7">
-        <v>4884.101755119999</v>
+        <v>881.3751837000001</v>
       </c>
       <c r="W15" s="8">
-        <v>72586.5</v>
+        <v>10912.56</v>
       </c>
       <c r="X15" s="7">
-        <v>33873.4338495</v>
+        <v>5067.43999545984</v>
       </c>
       <c r="Y15" s="7">
-        <v>55329.24538833999</v>
+        <v>13749.06787502131</v>
       </c>
     </row>
     <row r="18" spans="13:18">
       <c r="M18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="9">
+        <v>150</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>38</v>
+      </c>
+      <c r="R18" s="10">
+        <v>188000.1094897843</v>
+      </c>
+    </row>
+    <row r="19" spans="13:18">
+      <c r="Q19" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="9">
-        <v>153</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>43</v>
-      </c>
-      <c r="R18" s="10">
-        <v>676679.25123173</v>
-      </c>
-    </row>
-    <row r="19" spans="13:18">
-      <c r="M19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="9">
-        <v>153</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>44</v>
-      </c>
       <c r="R19" s="10">
-        <v>653502.1838868</v>
+        <v>208128.5769721167</v>
       </c>
     </row>
     <row r="21" spans="13:18">
       <c r="M21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N21" s="9">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="13:18">
-      <c r="M22" t="s">
-        <v>42</v>
-      </c>
-      <c r="N22" s="9">
-        <v>150</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3953,397 +3942,628 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="0.140625" customWidth="1"/>
+    <col min="1" max="10" width="0.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>140.28</v>
+        <v>108.4368</v>
       </c>
       <c r="C2">
-        <v>122.22</v>
+        <v>150</v>
       </c>
       <c r="D2">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E2">
-        <v>153</v>
-      </c>
-      <c r="F2">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G2">
-        <v>145</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>157.5</v>
-      </c>
-      <c r="I2">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>117302.2122811392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>137.76</v>
+        <v>87.9696</v>
       </c>
       <c r="C3">
-        <v>129.78</v>
+        <v>150</v>
       </c>
       <c r="D3">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E3">
-        <v>153</v>
-      </c>
-      <c r="F3">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G3">
-        <v>145</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>157.5</v>
-      </c>
-      <c r="I3">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>113465.8679611392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>142.8</v>
+        <v>88.1664</v>
       </c>
       <c r="C4">
-        <v>127.26</v>
+        <v>150</v>
       </c>
       <c r="D4">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E4">
-        <v>153</v>
-      </c>
-      <c r="F4">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G4">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="H4">
-        <v>157.5</v>
-      </c>
-      <c r="I4">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>109629.5236411392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>136.08</v>
+        <v>80.688</v>
       </c>
       <c r="C5">
-        <v>124.32</v>
+        <v>150</v>
       </c>
       <c r="D5">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E5">
-        <v>153</v>
-      </c>
-      <c r="F5">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G5">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>157.5</v>
-      </c>
-      <c r="I5">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>105793.1793211392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>138.6</v>
+        <v>110.208</v>
       </c>
       <c r="C6">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="D6">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E6">
-        <v>153</v>
-      </c>
-      <c r="F6">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G6">
-        <v>145</v>
+        <v>25</v>
       </c>
       <c r="H6">
-        <v>157.5</v>
-      </c>
-      <c r="I6">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>101956.8350011392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>132.72</v>
+        <v>137.1696</v>
       </c>
       <c r="C7">
-        <v>123.9</v>
+        <v>150</v>
       </c>
       <c r="D7">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E7">
-        <v>153</v>
-      </c>
-      <c r="F7">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G7">
-        <v>145</v>
+        <v>30</v>
       </c>
       <c r="H7">
-        <v>157.5</v>
-      </c>
-      <c r="I7">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>98120.4906811392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>137.76</v>
+        <v>137.3664</v>
       </c>
       <c r="C8">
-        <v>124.74</v>
+        <v>150</v>
       </c>
       <c r="D8">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E8">
-        <v>153</v>
-      </c>
-      <c r="F8">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G8">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="H8">
-        <v>157.5</v>
-      </c>
-      <c r="I8">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>94284.14636113921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>153.3</v>
+        <v>138.3504</v>
       </c>
       <c r="C9">
-        <v>151.62</v>
+        <v>150</v>
       </c>
       <c r="D9">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E9">
-        <v>153</v>
-      </c>
-      <c r="F9">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G9">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="H9">
-        <v>157.5</v>
-      </c>
-      <c r="I9">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>90447.80204113921</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>154.98</v>
+        <v>106.8624</v>
       </c>
       <c r="C10">
-        <v>140.7</v>
+        <v>150</v>
       </c>
       <c r="D10">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E10">
-        <v>153</v>
-      </c>
-      <c r="F10">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G10">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="H10">
-        <v>157.5</v>
-      </c>
-      <c r="I10">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>86611.4577211392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>157.5</v>
+        <v>75.9648</v>
       </c>
       <c r="C11">
-        <v>147.42</v>
+        <v>150</v>
       </c>
       <c r="D11">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E11">
-        <v>153</v>
-      </c>
-      <c r="F11">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G11">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="H11">
-        <v>157.5</v>
-      </c>
-      <c r="I11">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>82775.1134011392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>162.96</v>
+        <v>95.6448</v>
       </c>
       <c r="C12">
-        <v>147.42</v>
+        <v>150</v>
       </c>
       <c r="D12">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E12">
-        <v>153</v>
-      </c>
-      <c r="F12">
-        <v>150</v>
+        <v>110.25</v>
       </c>
       <c r="G12">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="H12">
-        <v>157.5</v>
-      </c>
-      <c r="I12">
-        <v>152.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>78938.76908113919</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>157.08</v>
+        <v>96.23520000000001</v>
       </c>
       <c r="C13">
-        <v>148.68</v>
+        <v>150</v>
       </c>
       <c r="D13">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E13">
-        <v>153</v>
-      </c>
-      <c r="F13">
+        <v>110.25</v>
+      </c>
+      <c r="G13">
+        <v>60</v>
+      </c>
+      <c r="H13">
+        <v>75102.42476113921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="G14">
+        <v>65</v>
+      </c>
+      <c r="H14">
+        <v>71266.0804411392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="G15">
+        <v>70</v>
+      </c>
+      <c r="H15">
+        <v>67429.7361211392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16">
+        <v>63531.7033844736</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10">
+      <c r="G17">
+        <v>80</v>
+      </c>
+      <c r="H17">
+        <v>60100.0678146048</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10">
+      <c r="G18">
+        <v>85</v>
+      </c>
+      <c r="H18">
+        <v>56808.4843880448</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19">
+        <v>90</v>
+      </c>
+      <c r="H19">
+        <v>54694.14715514881</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10">
+      <c r="G20">
+        <v>95</v>
+      </c>
+      <c r="H20">
+        <v>52655.7695397888</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10">
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>51636.58073210881</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10">
+      <c r="G22">
+        <v>105</v>
+      </c>
+      <c r="H22">
+        <v>50005.67403479041</v>
+      </c>
+      <c r="J22">
+        <v>50005.67403479041</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10">
+      <c r="G23">
+        <v>110</v>
+      </c>
+      <c r="H23">
+        <v>50155.9564296192</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10">
+      <c r="G24">
+        <v>115</v>
+      </c>
+      <c r="H24">
+        <v>50628.84980613121</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10">
+      <c r="G25">
+        <v>120</v>
+      </c>
+      <c r="H25">
+        <v>51108.3928461312</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10">
+      <c r="G26">
+        <v>125</v>
+      </c>
+      <c r="H26">
+        <v>51587.9358861312</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10">
+      <c r="G27">
+        <v>130</v>
+      </c>
+      <c r="H27">
+        <v>52067.4789261312</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10">
+      <c r="G28">
+        <v>135</v>
+      </c>
+      <c r="H28">
+        <v>52042.77286871041</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10">
+      <c r="G29">
+        <v>140</v>
+      </c>
+      <c r="H29">
+        <v>53708.82048000001</v>
+      </c>
+    </row>
+    <row r="30" spans="7:10">
+      <c r="G30">
+        <v>145</v>
+      </c>
+      <c r="H30">
+        <v>55626.99264</v>
+      </c>
+    </row>
+    <row r="31" spans="7:10">
+      <c r="G31">
         <v>150</v>
       </c>
-      <c r="G13">
-        <v>145</v>
-      </c>
-      <c r="H13">
-        <v>157.5</v>
-      </c>
-      <c r="I13">
-        <v>152.25</v>
+      <c r="H31">
+        <v>57545.1648</v>
+      </c>
+      <c r="I31">
+        <v>57545.1648</v>
+      </c>
+    </row>
+    <row r="32" spans="7:10">
+      <c r="G32">
+        <v>155</v>
+      </c>
+      <c r="H32">
+        <v>59463.33696</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8">
+      <c r="G33">
+        <v>160</v>
+      </c>
+      <c r="H33">
+        <v>61381.50912</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8">
+      <c r="G34">
+        <v>165</v>
+      </c>
+      <c r="H34">
+        <v>63299.68128</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8">
+      <c r="G35">
+        <v>170</v>
+      </c>
+      <c r="H35">
+        <v>65217.85344000001</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8">
+      <c r="G36">
+        <v>175</v>
+      </c>
+      <c r="H36">
+        <v>67136.02560000001</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8">
+      <c r="G37">
+        <v>180</v>
+      </c>
+      <c r="H37">
+        <v>69054.19776000001</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8">
+      <c r="G38">
+        <v>185</v>
+      </c>
+      <c r="H38">
+        <v>70972.36992</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8">
+      <c r="G39">
+        <v>190</v>
+      </c>
+      <c r="H39">
+        <v>72890.54208</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8">
+      <c r="G40">
+        <v>195</v>
+      </c>
+      <c r="H40">
+        <v>74808.71424</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8">
+      <c r="G41">
+        <v>200</v>
+      </c>
+      <c r="H41">
+        <v>76726.8864</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8">
+      <c r="G42">
+        <v>205</v>
+      </c>
+      <c r="H42">
+        <v>78645.05856</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8">
+      <c r="G43">
+        <v>210</v>
+      </c>
+      <c r="H43">
+        <v>80563.23072000001</v>
+      </c>
+    </row>
+    <row r="44" spans="7:8">
+      <c r="G44">
+        <v>215</v>
+      </c>
+      <c r="H44">
+        <v>82481.40288000001</v>
+      </c>
+    </row>
+    <row r="45" spans="7:8">
+      <c r="G45">
+        <v>220</v>
+      </c>
+      <c r="H45">
+        <v>84399.57504</v>
+      </c>
+    </row>
+    <row r="46" spans="7:8">
+      <c r="G46">
+        <v>225</v>
+      </c>
+      <c r="H46">
+        <v>86317.74720000001</v>
+      </c>
+    </row>
+    <row r="47" spans="7:8">
+      <c r="G47">
+        <v>230</v>
+      </c>
+      <c r="H47">
+        <v>88235.91936</v>
+      </c>
+    </row>
+    <row r="48" spans="7:8">
+      <c r="G48">
+        <v>235</v>
+      </c>
+      <c r="H48">
+        <v>90154.09152</v>
+      </c>
+    </row>
+    <row r="49" spans="7:8">
+      <c r="G49">
+        <v>240</v>
+      </c>
+      <c r="H49">
+        <v>92072.26368</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8">
+      <c r="G50">
+        <v>245</v>
+      </c>
+      <c r="H50">
+        <v>93990.43584000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correções na análise por fatura
</commit_message>
<xml_diff>
--- a/arquivos/Teste.xlsx
+++ b/arquivos/Teste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
   <si>
     <t>Mês</t>
   </si>
@@ -57,6 +57,9 @@
     <t>DEZ/23</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Demanda Registrada na Ponta</t>
   </si>
   <si>
@@ -156,28 +159,31 @@
     <t>Azul</t>
   </si>
   <si>
-    <t>Utilizada FP</t>
-  </si>
-  <si>
-    <t>Utilizada P</t>
-  </si>
-  <si>
-    <t>Contratada FP - 153 kW</t>
-  </si>
-  <si>
-    <t>Contratada P - 153 kW</t>
-  </si>
-  <si>
-    <t>Proposta FP - 150 kW</t>
-  </si>
-  <si>
-    <t>Proposta P - 145 kW</t>
-  </si>
-  <si>
-    <t>Proposta + Tolerância de 5% (FP)</t>
-  </si>
-  <si>
-    <t>Proposta + Tolerância de 5% (P)</t>
+    <t>Utilizada</t>
+  </si>
+  <si>
+    <t>Contratada - 153 kW</t>
+  </si>
+  <si>
+    <t>Proposta - 135 kW</t>
+  </si>
+  <si>
+    <t>Proposta + Tolerância de 5%</t>
+  </si>
+  <si>
+    <t>Custo</t>
+  </si>
+  <si>
+    <t>Demandas Contratadas</t>
+  </si>
+  <si>
+    <t>Custos Anuais</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
   </si>
   <si>
     <t>Economia Estimada</t>
@@ -291,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -309,6 +315,18 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -427,40 +445,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4315.5976059</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3852.2527284</c:v>
+                  <c:v>2.3342583</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3470.7111957</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3839.6391015</c:v>
+                  <c:v>7.078305599999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3811.6927425</c:v>
+                  <c:v>2.5824306</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4444.1112936</c:v>
+                  <c:v>1.5393876</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4348.7160195</c:v>
+                  <c:v>2.2982913</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4775.5795689</c:v>
+                  <c:v>13.9947597</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4112.646615</c:v>
+                  <c:v>3.9959337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5998.4216019</c:v>
+                  <c:v>1.7695764</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4126.7312922</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3384.9838512</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -657,40 +675,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4259.3349589</c:v>
+                  <c:v>993.94507268</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4591.29333894</c:v>
+                  <c:v>957.7496983599999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3876.2297917</c:v>
+                  <c:v>1329.71731886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4736.55074326</c:v>
+                  <c:v>2035.83116982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3858.60140176</c:v>
+                  <c:v>1507.54130632</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4735.4402935</c:v>
+                  <c:v>1694.8900444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4765.70004946</c:v>
+                  <c:v>1182.95287558</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4808.108654579999</c:v>
+                  <c:v>729.03670672</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5225.637764339999</c:v>
+                  <c:v>1929.59153296</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5265.40244146</c:v>
+                  <c:v>1902.76227358</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5047.82699652</c:v>
+                  <c:v>2118.27545468</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4884.101755119999</c:v>
+                  <c:v>1589.82034568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -714,40 +732,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>31962.4488645</c:v>
+                  <c:v>5705.515170600001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32633.74359</c:v>
+                  <c:v>5466.73304676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29879.965227</c:v>
+                  <c:v>7468.82931588</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32496.544668</c:v>
+                  <c:v>9679.859943360001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32565.144129</c:v>
+                  <c:v>8058.8966796</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33055.140279</c:v>
+                  <c:v>7866.034194960001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32594.543898</c:v>
+                  <c:v>5707.811152560001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34593.72819</c:v>
+                  <c:v>3852.65772888</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34716.2272275</c:v>
+                  <c:v>9273.471136439999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37675.8039735</c:v>
+                  <c:v>11567.15711448</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35054.324571</c:v>
+                  <c:v>13835.58729096</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33873.4338495</c:v>
+                  <c:v>11332.96695456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -971,13 +989,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1385.4418154496</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>639.9803577600005</c:v>
+                  <c:v>1271.6332602624</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>512.9095590144008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1103,40 +1121,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>53140.07998734999</c:v>
+                  <c:v>13860.10025102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55086.30186711</c:v>
+                  <c:v>13482.3053221</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49586.23364305</c:v>
+                  <c:v>17071.2108243644</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55506.98194519</c:v>
+                  <c:v>21835.93724919</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52203.70853644</c:v>
+                  <c:v>18192.4884323248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56061.31273675</c:v>
+                  <c:v>18712.68500356</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55716.93268549</c:v>
+                  <c:v>14588.30404183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57985.01330517</c:v>
+                  <c:v>10989.82951456</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59765.05869915</c:v>
+                  <c:v>21021.52199668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63440.23088899</c:v>
+                  <c:v>27025.2161259244</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60509.37502902</c:v>
+                  <c:v>29950.63845677359</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>57678.02190802</c:v>
+                  <c:v>24280.3354600016</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,40 +1184,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>52280.7708684</c:v>
+                  <c:v>17625.55870828</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53284.02397394</c:v>
+                  <c:v>17350.58121012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49815.18206370001</c:v>
+                  <c:v>19882.8667496344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53292.08245626</c:v>
+                  <c:v>22641.78957818</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52482.73257576</c:v>
+                  <c:v>21830.3086334832</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53849.5676175</c:v>
+                  <c:v>20487.02270436</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53419.23099246</c:v>
+                  <c:v>17816.86249314</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56080.0023798</c:v>
+                  <c:v>15507.7929006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56160.84712628</c:v>
+                  <c:v>22145.7806207584</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59910.65219158</c:v>
+                  <c:v>28209.0670882344</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57597.84625278</c:v>
+                  <c:v>32906.20169732319</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55329.24538833999</c:v>
+                  <c:v>26353.1366157616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1292,7 +1310,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Demanda Contratada X Demanda Recomendada (FP)</a:t>
+              <a:t>Demanda Contratada X Demanda Recomendada</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1312,7 +1330,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Utilizada FP</c:v>
+                  <c:v>Utilizada</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1378,40 +1396,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>140.28</c:v>
+                  <c:v>101.1552</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>137.76</c:v>
+                  <c:v>106.272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142.8</c:v>
+                  <c:v>139.9248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136.08</c:v>
+                  <c:v>134.6112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138.6</c:v>
+                  <c:v>135.2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>132.72</c:v>
+                  <c:v>103.5168</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137.76</c:v>
+                  <c:v>95.44799999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153.3</c:v>
+                  <c:v>67.1088</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>154.98</c:v>
+                  <c:v>123.984</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>157.5</c:v>
+                  <c:v>174.5616</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>162.96</c:v>
+                  <c:v>172.7904</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>157.08</c:v>
+                  <c:v>160.9824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1423,11 +1441,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$D$1</c:f>
+              <c:f>'Recomendação'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Contratada FP - 153 kW</c:v>
+                  <c:v>Contratada - 153 kW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1444,7 +1462,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$D$2:$D$13</c:f>
+              <c:f>'Recomendação'!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1493,11 +1511,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$F$1</c:f>
+              <c:f>'Recomendação'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Proposta FP - 150 kW</c:v>
+                  <c:v>Proposta - 135 kW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1514,45 +1532,45 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$F$2:$F$13</c:f>
+              <c:f>'Recomendação'!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>150</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1563,11 +1581,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$H$1</c:f>
+              <c:f>'Recomendação'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Proposta + Tolerância de 5% (FP)</c:v>
+                  <c:v>Proposta + Tolerância de 5%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1585,45 +1603,45 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$H$2:$H$13</c:f>
+              <c:f>'Recomendação'!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>157.5</c:v>
+                  <c:v>141.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1714,7 +1732,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Demanda Contratada X Demanda Recomendada (P)</a:t>
+              <a:t>Custo Anual X Demanda Contratada</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1730,11 +1748,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$C$1</c:f>
+              <c:f>'Recomendação'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Utilizada P</c:v>
+                  <c:v>Custos Anuais</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1750,90 +1768,283 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'Recomendação'!$A$2:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
+            <c:numRef>
+              <c:f>'Recomendação'!$G$2:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>JAN/23</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEV/23</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR/23</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ABR/23</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>MAI/23</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>JUN/23</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>JUL/23</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AGO/23</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SET/23</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>OUT/23</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>NOV/23</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>DEZ/23</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$C$2:$C$13</c:f>
+              <c:f>'Recomendação'!$H$2:$H$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>122.22</c:v>
+                  <c:v>119086.1570627712</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129.78</c:v>
+                  <c:v>115230.8537027712</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127.26</c:v>
+                  <c:v>111375.5503427712</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>124.32</c:v>
+                  <c:v>107520.2469827712</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>126</c:v>
+                  <c:v>103664.9436227712</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>123.9</c:v>
+                  <c:v>99809.64026277119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124.74</c:v>
+                  <c:v>95818.8358406784</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>151.62</c:v>
+                  <c:v>92377.69486963199</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140.7</c:v>
+                  <c:v>89004.304429632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>147.42</c:v>
+                  <c:v>85630.913989632</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>147.42</c:v>
+                  <c:v>82257.52354963199</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>148.68</c:v>
+                  <c:v>78884.13310963199</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75481.95640454399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72275.886130368</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70116.40220832</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68629.79723270399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67184.058472704</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65482.3275696</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>64390.505658048</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>62796.1578045312</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62170.9304076288</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>62488.14476808959</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>62970.0576880896</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>63451.97060808959</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>63549.48408107519</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>64352.67228107519</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64784.3634493056</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>65776.35870585599</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67467.8088</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>69395.46047999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>71323.11215999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>73250.76384</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>75178.41552</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>77106.06719999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>79033.71888</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>80961.37056</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82889.02223999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>84816.67391999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>86744.3256</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>88671.97727999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90599.62896</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>92527.28064</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>94454.93231999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>96382.584</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,66 +2056,37 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$E$1</c:f>
+              <c:f>'Recomendação'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Contratada P - 153 kW</c:v>
+                  <c:v>Column3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="C0504D"/>
-              </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="R$ #,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$E$2:$E$13</c:f>
+              <c:f>'Recomendação'!$I$2:$I$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>153</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>153</c:v>
+                <c:ptCount val="44"/>
+                <c:pt idx="24">
+                  <c:v>63549.48408107519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1915,137 +2097,37 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Recomendação'!$G$1</c:f>
+              <c:f>'Recomendação'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Proposta P - 145 kW</c:v>
+                  <c:v>Column4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="R$ #,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$G$2:$G$13</c:f>
+              <c:f>'Recomendação'!$J$2:$J$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>145</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Recomendação'!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Proposta + Tolerância de 5% (P)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="lgDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Recomendação'!$I$2:$I$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>152.25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>152.25</c:v>
+                <c:ptCount val="44"/>
+                <c:pt idx="20">
+                  <c:v>62170.9304076288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2061,7 +2143,36 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Demanda</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="50060002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -2086,14 +2197,14 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Demanda - kW</a:t>
+                  <a:t>Custo Anual</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="R$ #,##0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060001"/>
         <c:crosses val="autoZero"/>
@@ -2287,13 +2398,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2317,18 +2428,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0">
-  <autoFilter ref="A1:I13"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Mês"/>
-    <tableColumn id="2" name="Utilizada FP"/>
-    <tableColumn id="3" name="Utilizada P"/>
-    <tableColumn id="4" name="Contratada FP - 153 kW"/>
-    <tableColumn id="5" name="Contratada P - 153 kW"/>
-    <tableColumn id="6" name="Proposta FP - 150 kW"/>
-    <tableColumn id="7" name="Proposta P - 145 kW"/>
-    <tableColumn id="8" name="Proposta + Tolerância de 5% (FP)"/>
-    <tableColumn id="9" name="Proposta + Tolerância de 5% (P)"/>
+    <tableColumn id="2" name="Utilizada"/>
+    <tableColumn id="3" name="Contratada - 153 kW"/>
+    <tableColumn id="4" name="Proposta - 135 kW"/>
+    <tableColumn id="5" name="Proposta + Tolerância de 5%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="G1:J45" totalsRowShown="0">
+  <autoFilter ref="G1:J45"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Demandas Contratadas"/>
+    <tableColumn id="2" name="Custos Anuais"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2619,7 +2739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2633,52 +2753,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2686,13 +2806,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>122.22</v>
+        <v>64.1568</v>
       </c>
       <c r="C2" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D2" s="3">
-        <v>140.28</v>
+        <v>101.1552</v>
       </c>
       <c r="E2" s="4">
         <v>4915.511783999999</v>
@@ -2710,22 +2830,22 @@
         <v>0</v>
       </c>
       <c r="J2" s="5">
-        <v>6443.95</v>
+        <v>1503.74</v>
       </c>
       <c r="K2" s="4">
-        <v>4259.3349589</v>
+        <v>993.94507268</v>
       </c>
       <c r="L2" s="5">
-        <v>68491.5</v>
+        <v>12226.2</v>
       </c>
       <c r="M2" s="4">
-        <v>31962.4488645</v>
+        <v>5705.515170600001</v>
       </c>
       <c r="N2" s="6">
-        <v>11998.77</v>
+        <v>0</v>
       </c>
       <c r="O2" s="4">
-        <v>4315.5976059</v>
+        <v>0</v>
       </c>
       <c r="P2" s="3">
         <v>0</v>
@@ -2739,13 +2859,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>129.78</v>
+        <v>66.5184</v>
       </c>
       <c r="C3" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D3" s="3">
-        <v>137.76</v>
+        <v>106.272</v>
       </c>
       <c r="E3" s="4">
         <v>4915.511783999999</v>
@@ -2763,22 +2883,22 @@
         <v>0</v>
       </c>
       <c r="J3" s="5">
-        <v>6946.17</v>
+        <v>1448.98</v>
       </c>
       <c r="K3" s="4">
-        <v>4591.29333894</v>
+        <v>957.7496983599999</v>
       </c>
       <c r="L3" s="5">
-        <v>69930</v>
+        <v>11714.52</v>
       </c>
       <c r="M3" s="4">
-        <v>32633.74359</v>
+        <v>5466.73304676</v>
       </c>
       <c r="N3" s="6">
-        <v>10710.52</v>
+        <v>6.49</v>
       </c>
       <c r="O3" s="4">
-        <v>3852.2527284</v>
+        <v>2.3342583</v>
       </c>
       <c r="P3" s="3">
         <v>0</v>
@@ -2792,13 +2912,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>127.26</v>
+        <v>77.1456</v>
       </c>
       <c r="C4" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D4" s="3">
-        <v>142.8</v>
+        <v>139.9248</v>
       </c>
       <c r="E4" s="4">
         <v>4915.511783999999</v>
@@ -2816,22 +2936,22 @@
         <v>0</v>
       </c>
       <c r="J4" s="5">
-        <v>5864.35</v>
+        <v>2011.73</v>
       </c>
       <c r="K4" s="4">
-        <v>3876.2297917</v>
+        <v>1329.71731886</v>
       </c>
       <c r="L4" s="5">
-        <v>64029</v>
+        <v>16004.76</v>
       </c>
       <c r="M4" s="4">
-        <v>29879.965227</v>
+        <v>7468.82931588</v>
       </c>
       <c r="N4" s="6">
-        <v>9649.709999999999</v>
+        <v>0</v>
       </c>
       <c r="O4" s="4">
-        <v>3470.7111957</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
         <v>0</v>
@@ -2845,13 +2965,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>124.32</v>
+        <v>84.624</v>
       </c>
       <c r="C5" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D5" s="3">
-        <v>136.08</v>
+        <v>134.6112</v>
       </c>
       <c r="E5" s="4">
         <v>4915.511783999999</v>
@@ -2869,22 +2989,22 @@
         <v>0</v>
       </c>
       <c r="J5" s="5">
-        <v>7165.93</v>
+        <v>3080.01</v>
       </c>
       <c r="K5" s="4">
-        <v>4736.55074326</v>
+        <v>2035.83116982</v>
       </c>
       <c r="L5" s="5">
-        <v>69636</v>
+        <v>20742.72</v>
       </c>
       <c r="M5" s="4">
-        <v>32496.544668</v>
+        <v>9679.859943360001</v>
       </c>
       <c r="N5" s="6">
-        <v>10675.45</v>
+        <v>19.68</v>
       </c>
       <c r="O5" s="4">
-        <v>3839.6391015</v>
+        <v>7.078305599999999</v>
       </c>
       <c r="P5" s="3">
         <v>0</v>
@@ -2898,13 +3018,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>126</v>
+        <v>90.7248</v>
       </c>
       <c r="C6" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D6" s="3">
-        <v>138.6</v>
+        <v>135.2016</v>
       </c>
       <c r="E6" s="4">
         <v>4915.511783999999</v>
@@ -2922,22 +3042,22 @@
         <v>0</v>
       </c>
       <c r="J6" s="5">
-        <v>5837.68</v>
+        <v>2280.76</v>
       </c>
       <c r="K6" s="4">
-        <v>3858.60140176</v>
+        <v>1507.54130632</v>
       </c>
       <c r="L6" s="5">
-        <v>69783</v>
+        <v>17269.2</v>
       </c>
       <c r="M6" s="4">
-        <v>32565.144129</v>
+        <v>8058.8966796</v>
       </c>
       <c r="N6" s="6">
-        <v>10597.75</v>
+        <v>7.18</v>
       </c>
       <c r="O6" s="4">
-        <v>3811.6927425</v>
+        <v>2.5824306</v>
       </c>
       <c r="P6" s="3">
         <v>0</v>
@@ -2951,13 +3071,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>123.9</v>
+        <v>71.0448</v>
       </c>
       <c r="C7" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D7" s="3">
-        <v>132.72</v>
+        <v>103.5168</v>
       </c>
       <c r="E7" s="4">
         <v>4915.511783999999</v>
@@ -2975,22 +3095,22 @@
         <v>0</v>
       </c>
       <c r="J7" s="5">
-        <v>7164.25</v>
+        <v>2564.2</v>
       </c>
       <c r="K7" s="4">
-        <v>4735.4402935</v>
+        <v>1694.8900444</v>
       </c>
       <c r="L7" s="5">
-        <v>70833</v>
+        <v>16855.92</v>
       </c>
       <c r="M7" s="4">
-        <v>33055.140279</v>
+        <v>7866.034194960001</v>
       </c>
       <c r="N7" s="6">
-        <v>12356.08</v>
+        <v>4.28</v>
       </c>
       <c r="O7" s="4">
-        <v>4444.1112936</v>
+        <v>1.5393876</v>
       </c>
       <c r="P7" s="3">
         <v>0</v>
@@ -3004,13 +3124,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>124.74</v>
+        <v>56.4816</v>
       </c>
       <c r="C8" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D8" s="3">
-        <v>137.76</v>
+        <v>95.44799999999999</v>
       </c>
       <c r="E8" s="4">
         <v>4915.511783999999</v>
@@ -3028,22 +3148,22 @@
         <v>0</v>
       </c>
       <c r="J8" s="5">
-        <v>7210.03</v>
+        <v>1789.69</v>
       </c>
       <c r="K8" s="4">
-        <v>4765.70004946</v>
+        <v>1182.95287558</v>
       </c>
       <c r="L8" s="5">
-        <v>69846</v>
+        <v>12231.12</v>
       </c>
       <c r="M8" s="4">
-        <v>32594.543898</v>
+        <v>5707.811152560001</v>
       </c>
       <c r="N8" s="6">
-        <v>12090.85</v>
+        <v>6.39</v>
       </c>
       <c r="O8" s="4">
-        <v>4348.7160195</v>
+        <v>2.2982913</v>
       </c>
       <c r="P8" s="3">
         <v>0</v>
@@ -3057,16 +3177,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>151.62</v>
+        <v>49.7904</v>
       </c>
       <c r="C9" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D9" s="3">
-        <v>153.3</v>
+        <v>67.1088</v>
       </c>
       <c r="E9" s="4">
-        <v>4925.1500424</v>
+        <v>4915.511783999999</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -3081,22 +3201,22 @@
         <v>0</v>
       </c>
       <c r="J9" s="5">
-        <v>7274.19</v>
+        <v>1102.96</v>
       </c>
       <c r="K9" s="4">
-        <v>4808.108654579999</v>
+        <v>729.03670672</v>
       </c>
       <c r="L9" s="5">
-        <v>74130</v>
+        <v>8255.76</v>
       </c>
       <c r="M9" s="4">
-        <v>34593.72819</v>
+        <v>3852.65772888</v>
       </c>
       <c r="N9" s="6">
-        <v>13277.67</v>
+        <v>38.91</v>
       </c>
       <c r="O9" s="4">
-        <v>4775.5795689</v>
+        <v>13.9947597</v>
       </c>
       <c r="P9" s="3">
         <v>0</v>
@@ -3110,16 +3230,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>140.7</v>
+        <v>85.2144</v>
       </c>
       <c r="C10" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D10" s="3">
-        <v>154.98</v>
+        <v>123.984</v>
       </c>
       <c r="E10" s="4">
-        <v>4979.124289439999</v>
+        <v>4915.511783999999</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -3134,22 +3254,22 @@
         <v>0</v>
       </c>
       <c r="J10" s="5">
-        <v>7905.87</v>
+        <v>2919.28</v>
       </c>
       <c r="K10" s="4">
-        <v>5225.637764339999</v>
+        <v>1929.59153296</v>
       </c>
       <c r="L10" s="5">
-        <v>74392.5</v>
+        <v>19871.88</v>
       </c>
       <c r="M10" s="4">
-        <v>34716.2272275</v>
+        <v>9273.471136439999</v>
       </c>
       <c r="N10" s="6">
-        <v>11434.5</v>
+        <v>11.11</v>
       </c>
       <c r="O10" s="4">
-        <v>4112.646615</v>
+        <v>3.9959337</v>
       </c>
       <c r="P10" s="3">
         <v>0</v>
@@ -3163,16 +3283,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>147.42</v>
+        <v>81.86879999999999</v>
       </c>
       <c r="C11" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D11" s="3">
-        <v>157.5</v>
+        <v>174.5616</v>
       </c>
       <c r="E11" s="4">
-        <v>5060.08566</v>
+        <v>5608.232691724799</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -3181,28 +3301,28 @@
         <v>0</v>
       </c>
       <c r="H11" s="3">
-        <v>0</v>
+        <v>21.5616</v>
       </c>
       <c r="I11" s="4">
-        <v>0</v>
+        <v>1385.4418154496</v>
       </c>
       <c r="J11" s="5">
-        <v>7966.03</v>
+        <v>2878.69</v>
       </c>
       <c r="K11" s="4">
-        <v>5265.40244146</v>
+        <v>1902.76227358</v>
       </c>
       <c r="L11" s="5">
-        <v>80734.5</v>
+        <v>24786.96</v>
       </c>
       <c r="M11" s="4">
-        <v>37675.8039735</v>
+        <v>11567.15711448</v>
       </c>
       <c r="N11" s="6">
-        <v>16677.57</v>
+        <v>4.92</v>
       </c>
       <c r="O11" s="4">
-        <v>5998.4216019</v>
+        <v>1.7695764</v>
       </c>
       <c r="P11" s="3">
         <v>0</v>
@@ -3216,16 +3336,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>147.42</v>
+        <v>95.2512</v>
       </c>
       <c r="C12" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D12" s="3">
-        <v>162.96</v>
+        <v>172.7904</v>
       </c>
       <c r="E12" s="4">
-        <v>5235.50196288</v>
+        <v>5551.3284141312</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -3234,28 +3354,28 @@
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <v>9.960000000000008</v>
+        <v>19.79040000000001</v>
       </c>
       <c r="I12" s="4">
-        <v>639.9803577600005</v>
+        <v>1271.6332602624</v>
       </c>
       <c r="J12" s="5">
-        <v>7636.86</v>
+        <v>3204.74</v>
       </c>
       <c r="K12" s="4">
-        <v>5047.82699652</v>
+        <v>2118.27545468</v>
       </c>
       <c r="L12" s="5">
-        <v>75117</v>
+        <v>29647.92</v>
       </c>
       <c r="M12" s="4">
-        <v>35054.324571</v>
+        <v>13835.58729096</v>
       </c>
       <c r="N12" s="6">
-        <v>11473.66</v>
+        <v>0</v>
       </c>
       <c r="O12" s="4">
-        <v>4126.7312922</v>
+        <v>0</v>
       </c>
       <c r="P12" s="3">
         <v>0</v>
@@ -3269,16 +3389,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>148.68</v>
+        <v>61.992</v>
       </c>
       <c r="C13" s="4">
         <v>11859.987933</v>
       </c>
       <c r="D13" s="3">
-        <v>157.08</v>
+        <v>160.9824</v>
       </c>
       <c r="E13" s="4">
-        <v>5046.59209824</v>
+        <v>5171.9665635072</v>
       </c>
       <c r="F13" s="3">
         <v>0</v>
@@ -3287,33 +3407,86 @@
         <v>0</v>
       </c>
       <c r="H13" s="3">
-        <v>0</v>
+        <v>7.982400000000013</v>
       </c>
       <c r="I13" s="4">
-        <v>0</v>
+        <v>512.9095590144008</v>
       </c>
       <c r="J13" s="5">
-        <v>7389.16</v>
+        <v>2405.24</v>
       </c>
       <c r="K13" s="4">
-        <v>4884.101755119999</v>
+        <v>1589.82034568</v>
       </c>
       <c r="L13" s="5">
-        <v>72586.5</v>
+        <v>24285.12</v>
       </c>
       <c r="M13" s="4">
-        <v>33873.4338495</v>
+        <v>11332.96695456</v>
       </c>
       <c r="N13" s="6">
-        <v>9411.360000000001</v>
+        <v>0</v>
       </c>
       <c r="O13" s="4">
-        <v>3384.9838512</v>
+        <v>0</v>
       </c>
       <c r="P13" s="3">
         <v>0</v>
       </c>
       <c r="Q13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>884.8127999999999</v>
+      </c>
+      <c r="C14" s="8">
+        <v>142319.855196</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1515.5568</v>
+      </c>
+      <c r="E14" s="8">
+        <v>60571.13372536319</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>49.33440000000002</v>
+      </c>
+      <c r="I14" s="8">
+        <v>3169.984634726401</v>
+      </c>
+      <c r="J14" s="9">
+        <v>27190.02</v>
+      </c>
+      <c r="K14" s="8">
+        <v>17972.11379964</v>
+      </c>
+      <c r="L14" s="9">
+        <v>213892.08</v>
+      </c>
+      <c r="M14" s="8">
+        <v>99815.51972904</v>
+      </c>
+      <c r="N14" s="10">
+        <v>98.95999999999999</v>
+      </c>
+      <c r="O14" s="8">
+        <v>35.59294319999999</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3325,7 +3498,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3339,48 +3512,48 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3390,37 +3563,37 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -3428,118 +3601,118 @@
     <row r="3" spans="1:25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="P3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="R3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="T3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
-        <v>140.28</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
-        <v>6443.95</v>
-      </c>
-      <c r="G4" s="8">
-        <v>16358.50192285</v>
-      </c>
-      <c r="H4" s="9">
-        <v>68491.5</v>
-      </c>
-      <c r="I4" s="8">
-        <v>31962.4488645</v>
-      </c>
-      <c r="J4" s="8">
-        <v>53140.07998734999</v>
+      <c r="B4" s="11">
+        <v>101.1552</v>
+      </c>
+      <c r="C4" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1503.74</v>
+      </c>
+      <c r="G4" s="12">
+        <v>3817.36880042</v>
+      </c>
+      <c r="H4" s="13">
+        <v>12226.2</v>
+      </c>
+      <c r="I4" s="12">
+        <v>5705.515170600001</v>
+      </c>
+      <c r="J4" s="12">
+        <v>13860.10025102</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="3">
-        <v>122.22</v>
+        <v>64.1568</v>
       </c>
       <c r="N4" s="4">
-        <v>11239.857845</v>
+        <v>6588.882185</v>
       </c>
       <c r="O4" s="3">
-        <v>140.28</v>
+        <v>101.1552</v>
       </c>
       <c r="P4" s="4">
-        <v>4819.129199999999</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q4" s="3">
         <v>0</v>
@@ -3554,66 +3727,66 @@
         <v>0</v>
       </c>
       <c r="U4" s="5">
-        <v>6443.95</v>
+        <v>1503.74</v>
       </c>
       <c r="V4" s="4">
-        <v>4259.3349589</v>
+        <v>993.94507268</v>
       </c>
       <c r="W4" s="5">
-        <v>68491.5</v>
+        <v>12226.2</v>
       </c>
       <c r="X4" s="4">
-        <v>31962.4488645</v>
+        <v>5705.515170600001</v>
       </c>
       <c r="Y4" s="4">
-        <v>52280.7708684</v>
+        <v>17625.55870828</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
-        <v>137.76</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9">
-        <v>6946.17</v>
-      </c>
-      <c r="G5" s="8">
-        <v>17633.42907711</v>
-      </c>
-      <c r="H5" s="9">
-        <v>69930</v>
-      </c>
-      <c r="I5" s="8">
-        <v>32633.74359</v>
-      </c>
-      <c r="J5" s="8">
-        <v>55086.30186711</v>
+      <c r="B5" s="11">
+        <v>106.272</v>
+      </c>
+      <c r="C5" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1448.98</v>
+      </c>
+      <c r="G5" s="12">
+        <v>3678.35599534</v>
+      </c>
+      <c r="H5" s="13">
+        <v>11714.52</v>
+      </c>
+      <c r="I5" s="12">
+        <v>5466.73304676</v>
+      </c>
+      <c r="J5" s="12">
+        <v>13482.3053221</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M5" s="3">
-        <v>129.78</v>
+        <v>66.5184</v>
       </c>
       <c r="N5" s="4">
-        <v>11239.857845</v>
+        <v>6588.882185</v>
       </c>
       <c r="O5" s="3">
-        <v>137.76</v>
+        <v>106.272</v>
       </c>
       <c r="P5" s="4">
-        <v>4819.129199999999</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q5" s="3">
         <v>0</v>
@@ -3628,66 +3801,66 @@
         <v>0</v>
       </c>
       <c r="U5" s="5">
-        <v>6946.17</v>
+        <v>1448.98</v>
       </c>
       <c r="V5" s="4">
-        <v>4591.29333894</v>
+        <v>957.7496983599999</v>
       </c>
       <c r="W5" s="5">
-        <v>69930</v>
+        <v>11714.52</v>
       </c>
       <c r="X5" s="4">
-        <v>32633.74359</v>
+        <v>5466.73304676</v>
       </c>
       <c r="Y5" s="4">
-        <v>53284.02397394</v>
+        <v>17350.58121012</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
-        <v>142.8</v>
-      </c>
-      <c r="C6" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9">
-        <v>5864.35</v>
-      </c>
-      <c r="G6" s="8">
-        <v>14887.13921605</v>
-      </c>
-      <c r="H6" s="9">
-        <v>64029</v>
-      </c>
-      <c r="I6" s="8">
-        <v>29879.965227</v>
-      </c>
-      <c r="J6" s="8">
-        <v>49586.23364305</v>
+      <c r="B6" s="11">
+        <v>139.9248</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4495.4379298944</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2011.73</v>
+      </c>
+      <c r="G6" s="12">
+        <v>5106.94357859</v>
+      </c>
+      <c r="H6" s="13">
+        <v>16004.76</v>
+      </c>
+      <c r="I6" s="12">
+        <v>7468.82931588</v>
+      </c>
+      <c r="J6" s="12">
+        <v>17071.2108243644</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="3">
-        <v>127.26</v>
+        <v>77.1456</v>
       </c>
       <c r="N6" s="4">
-        <v>11239.857845</v>
+        <v>6588.882185</v>
       </c>
       <c r="O6" s="3">
-        <v>142.8</v>
+        <v>139.9248</v>
       </c>
       <c r="P6" s="4">
-        <v>4819.129199999999</v>
+        <v>4495.4379298944</v>
       </c>
       <c r="Q6" s="3">
         <v>0</v>
@@ -3702,66 +3875,66 @@
         <v>0</v>
       </c>
       <c r="U6" s="5">
-        <v>5864.35</v>
+        <v>2011.73</v>
       </c>
       <c r="V6" s="4">
-        <v>3876.2297917</v>
+        <v>1329.71731886</v>
       </c>
       <c r="W6" s="5">
-        <v>64029</v>
+        <v>16004.76</v>
       </c>
       <c r="X6" s="4">
-        <v>29879.965227</v>
+        <v>7468.82931588</v>
       </c>
       <c r="Y6" s="4">
-        <v>49815.18206370001</v>
+        <v>19882.8667496344</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
-        <v>136.08</v>
-      </c>
-      <c r="C7" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9">
-        <v>7165.93</v>
-      </c>
-      <c r="G7" s="8">
-        <v>18191.30807719</v>
-      </c>
-      <c r="H7" s="9">
-        <v>69636</v>
-      </c>
-      <c r="I7" s="8">
-        <v>32496.544668</v>
-      </c>
-      <c r="J7" s="8">
-        <v>55506.98194519</v>
+      <c r="B7" s="11">
+        <v>134.6112</v>
+      </c>
+      <c r="C7" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>3080.01</v>
+      </c>
+      <c r="G7" s="12">
+        <v>7818.86102583</v>
+      </c>
+      <c r="H7" s="13">
+        <v>20742.72</v>
+      </c>
+      <c r="I7" s="12">
+        <v>9679.859943360001</v>
+      </c>
+      <c r="J7" s="12">
+        <v>21835.93724919</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M7" s="3">
-        <v>124.32</v>
+        <v>84.624</v>
       </c>
       <c r="N7" s="4">
-        <v>11239.857845</v>
+        <v>6588.882185</v>
       </c>
       <c r="O7" s="3">
-        <v>136.08</v>
+        <v>134.6112</v>
       </c>
       <c r="P7" s="4">
-        <v>4819.129199999999</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q7" s="3">
         <v>0</v>
@@ -3776,72 +3949,72 @@
         <v>0</v>
       </c>
       <c r="U7" s="5">
-        <v>7165.93</v>
+        <v>3080.01</v>
       </c>
       <c r="V7" s="4">
-        <v>4736.55074326</v>
+        <v>2035.83116982</v>
       </c>
       <c r="W7" s="5">
-        <v>69636</v>
+        <v>20742.72</v>
       </c>
       <c r="X7" s="4">
-        <v>32496.544668</v>
+        <v>9679.859943360001</v>
       </c>
       <c r="Y7" s="4">
-        <v>53292.08245626</v>
+        <v>22641.78957818</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
-        <v>138.6</v>
-      </c>
-      <c r="C8" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <v>5837.68</v>
-      </c>
-      <c r="G8" s="8">
-        <v>14819.43520744</v>
-      </c>
-      <c r="H8" s="9">
-        <v>69783</v>
-      </c>
-      <c r="I8" s="8">
-        <v>32565.144129</v>
-      </c>
-      <c r="J8" s="8">
-        <v>52203.70853644</v>
+      <c r="B8" s="11">
+        <v>135.2016</v>
+      </c>
+      <c r="C8" s="12">
+        <v>4343.6931896448</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>2280.76</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5789.898563080001</v>
+      </c>
+      <c r="H8" s="13">
+        <v>17269.2</v>
+      </c>
+      <c r="I8" s="12">
+        <v>8058.8966796</v>
+      </c>
+      <c r="J8" s="12">
+        <v>18192.4884323248</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M8" s="3">
-        <v>126</v>
+        <v>90.7248</v>
       </c>
       <c r="N8" s="4">
-        <v>11239.857845</v>
+        <v>7032.6472759728</v>
       </c>
       <c r="O8" s="3">
-        <v>138.6</v>
+        <v>135.2016</v>
       </c>
       <c r="P8" s="4">
-        <v>4819.129199999999</v>
+        <v>4343.6931896448</v>
       </c>
       <c r="Q8" s="3">
-        <v>0</v>
+        <v>5.724800000000002</v>
       </c>
       <c r="R8" s="4">
-        <v>0</v>
+        <v>887.5301819456002</v>
       </c>
       <c r="S8" s="3">
         <v>0</v>
@@ -3850,66 +4023,66 @@
         <v>0</v>
       </c>
       <c r="U8" s="5">
-        <v>5837.68</v>
+        <v>2280.76</v>
       </c>
       <c r="V8" s="4">
-        <v>3858.60140176</v>
+        <v>1507.54130632</v>
       </c>
       <c r="W8" s="5">
-        <v>69783</v>
+        <v>17269.2</v>
       </c>
       <c r="X8" s="4">
-        <v>32565.144129</v>
+        <v>8058.8966796</v>
       </c>
       <c r="Y8" s="4">
-        <v>52482.73257576</v>
+        <v>21830.3086334832</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7">
-        <v>132.72</v>
-      </c>
-      <c r="C9" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>7164.25</v>
-      </c>
-      <c r="G9" s="8">
-        <v>18187.04325775</v>
-      </c>
-      <c r="H9" s="9">
-        <v>70833</v>
-      </c>
-      <c r="I9" s="8">
-        <v>33055.140279</v>
-      </c>
-      <c r="J9" s="8">
-        <v>56061.31273675</v>
+      <c r="B9" s="11">
+        <v>103.5168</v>
+      </c>
+      <c r="C9" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>2564.2</v>
+      </c>
+      <c r="G9" s="12">
+        <v>6509.4345286</v>
+      </c>
+      <c r="H9" s="13">
+        <v>16855.92</v>
+      </c>
+      <c r="I9" s="12">
+        <v>7866.034194960001</v>
+      </c>
+      <c r="J9" s="12">
+        <v>18712.68500356</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M9" s="3">
-        <v>123.9</v>
+        <v>71.0448</v>
       </c>
       <c r="N9" s="4">
-        <v>11239.857845</v>
+        <v>6588.882185</v>
       </c>
       <c r="O9" s="3">
-        <v>132.72</v>
+        <v>103.5168</v>
       </c>
       <c r="P9" s="4">
-        <v>4819.129199999999</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q9" s="3">
         <v>0</v>
@@ -3924,66 +4097,66 @@
         <v>0</v>
       </c>
       <c r="U9" s="5">
-        <v>7164.25</v>
+        <v>2564.2</v>
       </c>
       <c r="V9" s="4">
-        <v>4735.4402935</v>
+        <v>1694.8900444</v>
       </c>
       <c r="W9" s="5">
-        <v>70833</v>
+        <v>16855.92</v>
       </c>
       <c r="X9" s="4">
-        <v>33055.140279</v>
+        <v>7866.034194960001</v>
       </c>
       <c r="Y9" s="4">
-        <v>53849.5676175</v>
+        <v>20487.02270436</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7">
-        <v>137.76</v>
-      </c>
-      <c r="C10" s="8">
-        <v>4819.129199999999</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <v>7210.03</v>
-      </c>
-      <c r="G10" s="8">
-        <v>18303.25958749</v>
-      </c>
-      <c r="H10" s="9">
-        <v>69846</v>
-      </c>
-      <c r="I10" s="8">
-        <v>32594.543898</v>
-      </c>
-      <c r="J10" s="8">
-        <v>55716.93268549</v>
+      <c r="B10" s="11">
+        <v>95.44799999999999</v>
+      </c>
+      <c r="C10" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1789.69</v>
+      </c>
+      <c r="G10" s="12">
+        <v>4543.27660927</v>
+      </c>
+      <c r="H10" s="13">
+        <v>12231.12</v>
+      </c>
+      <c r="I10" s="12">
+        <v>5707.811152560001</v>
+      </c>
+      <c r="J10" s="12">
+        <v>14588.30404183</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="3">
-        <v>124.74</v>
+        <v>56.4816</v>
       </c>
       <c r="N10" s="4">
-        <v>11239.857845</v>
+        <v>6588.882185</v>
       </c>
       <c r="O10" s="3">
-        <v>137.76</v>
+        <v>95.44799999999999</v>
       </c>
       <c r="P10" s="4">
-        <v>4819.129199999999</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q10" s="3">
         <v>0</v>
@@ -3998,66 +4171,66 @@
         <v>0</v>
       </c>
       <c r="U10" s="5">
-        <v>7210.03</v>
+        <v>1789.69</v>
       </c>
       <c r="V10" s="4">
-        <v>4765.70004946</v>
+        <v>1182.95287558</v>
       </c>
       <c r="W10" s="5">
-        <v>69846</v>
+        <v>12231.12</v>
       </c>
       <c r="X10" s="4">
-        <v>32594.543898</v>
+        <v>5707.811152560001</v>
       </c>
       <c r="Y10" s="4">
-        <v>53419.23099246</v>
+        <v>17816.86249314</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
-        <v>153.3</v>
-      </c>
-      <c r="C11" s="8">
-        <v>4925.1500424</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9">
-        <v>7274.19</v>
-      </c>
-      <c r="G11" s="8">
-        <v>18466.13507277</v>
-      </c>
-      <c r="H11" s="9">
-        <v>74130</v>
-      </c>
-      <c r="I11" s="8">
-        <v>34593.72819</v>
-      </c>
-      <c r="J11" s="8">
-        <v>57985.01330517</v>
+      <c r="B11" s="11">
+        <v>67.1088</v>
+      </c>
+      <c r="C11" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1102.96</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2799.95550568</v>
+      </c>
+      <c r="H11" s="13">
+        <v>8255.76</v>
+      </c>
+      <c r="I11" s="12">
+        <v>3852.65772888</v>
+      </c>
+      <c r="J11" s="12">
+        <v>10989.82951456</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M11" s="3">
-        <v>151.62</v>
+        <v>49.7904</v>
       </c>
       <c r="N11" s="4">
-        <v>11753.01549282</v>
+        <v>6588.882185</v>
       </c>
       <c r="O11" s="3">
-        <v>153.3</v>
+        <v>67.1088</v>
       </c>
       <c r="P11" s="4">
-        <v>4925.1500424</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q11" s="3">
         <v>0</v>
@@ -4072,66 +4245,66 @@
         <v>0</v>
       </c>
       <c r="U11" s="5">
-        <v>7274.19</v>
+        <v>1102.96</v>
       </c>
       <c r="V11" s="4">
-        <v>4808.108654579999</v>
+        <v>729.03670672</v>
       </c>
       <c r="W11" s="5">
-        <v>74130</v>
+        <v>8255.76</v>
       </c>
       <c r="X11" s="4">
-        <v>34593.72819</v>
+        <v>3852.65772888</v>
       </c>
       <c r="Y11" s="4">
-        <v>56080.0023798</v>
+        <v>15507.7929006</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
-        <v>154.98</v>
-      </c>
-      <c r="C12" s="8">
-        <v>4979.124289439999</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>7905.87</v>
-      </c>
-      <c r="G12" s="8">
-        <v>20069.70718221</v>
-      </c>
-      <c r="H12" s="9">
-        <v>74392.5</v>
-      </c>
-      <c r="I12" s="8">
-        <v>34716.2272275</v>
-      </c>
-      <c r="J12" s="8">
-        <v>59765.05869915</v>
+      <c r="B12" s="11">
+        <v>123.984</v>
+      </c>
+      <c r="C12" s="12">
+        <v>4337.21628</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2919.28</v>
+      </c>
+      <c r="G12" s="12">
+        <v>7410.834580240001</v>
+      </c>
+      <c r="H12" s="13">
+        <v>19871.88</v>
+      </c>
+      <c r="I12" s="12">
+        <v>9273.471136439999</v>
+      </c>
+      <c r="J12" s="12">
+        <v>21021.52199668</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M12" s="3">
-        <v>140.7</v>
+        <v>85.2144</v>
       </c>
       <c r="N12" s="4">
-        <v>11239.857845</v>
+        <v>6605.5016713584</v>
       </c>
       <c r="O12" s="3">
-        <v>154.98</v>
+        <v>123.984</v>
       </c>
       <c r="P12" s="4">
-        <v>4979.124289439999</v>
+        <v>4337.21628</v>
       </c>
       <c r="Q12" s="3">
         <v>0</v>
@@ -4146,66 +4319,66 @@
         <v>0</v>
       </c>
       <c r="U12" s="5">
-        <v>7905.87</v>
+        <v>2919.28</v>
       </c>
       <c r="V12" s="4">
-        <v>5225.637764339999</v>
+        <v>1929.59153296</v>
       </c>
       <c r="W12" s="5">
-        <v>74392.5</v>
+        <v>19871.88</v>
       </c>
       <c r="X12" s="4">
-        <v>34716.2272275</v>
+        <v>9273.471136439999</v>
       </c>
       <c r="Y12" s="4">
-        <v>56160.84712628</v>
+        <v>22145.7806207584</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7">
-        <v>157.5</v>
-      </c>
-      <c r="C13" s="8">
-        <v>5060.08566</v>
-      </c>
-      <c r="D13" s="7">
-        <v>7.5</v>
-      </c>
-      <c r="E13" s="8">
-        <v>481.91292</v>
-      </c>
-      <c r="F13" s="9">
-        <v>7966.03</v>
-      </c>
-      <c r="G13" s="8">
-        <v>20222.42833549</v>
-      </c>
-      <c r="H13" s="9">
-        <v>80734.5</v>
-      </c>
-      <c r="I13" s="8">
-        <v>37675.8039735</v>
-      </c>
-      <c r="J13" s="8">
-        <v>63440.23088899</v>
+      <c r="B13" s="11">
+        <v>174.5616</v>
+      </c>
+      <c r="C13" s="12">
+        <v>5608.232691724799</v>
+      </c>
+      <c r="D13" s="11">
+        <v>39.5616</v>
+      </c>
+      <c r="E13" s="12">
+        <v>2542.0328234496</v>
+      </c>
+      <c r="F13" s="13">
+        <v>2878.69</v>
+      </c>
+      <c r="G13" s="12">
+        <v>7307.79349627</v>
+      </c>
+      <c r="H13" s="13">
+        <v>24786.96</v>
+      </c>
+      <c r="I13" s="12">
+        <v>11567.15711448</v>
+      </c>
+      <c r="J13" s="12">
+        <v>27025.2161259244</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M13" s="3">
-        <v>147.42</v>
+        <v>81.86879999999999</v>
       </c>
       <c r="N13" s="4">
-        <v>11427.44719662</v>
+        <v>6588.882185</v>
       </c>
       <c r="O13" s="3">
-        <v>157.5</v>
+        <v>174.5616</v>
       </c>
       <c r="P13" s="4">
-        <v>5060.08566</v>
+        <v>5608.232691724799</v>
       </c>
       <c r="Q13" s="3">
         <v>0</v>
@@ -4214,146 +4387,146 @@
         <v>0</v>
       </c>
       <c r="S13" s="3">
-        <v>7.5</v>
+        <v>39.5616</v>
       </c>
       <c r="T13" s="4">
-        <v>481.91292</v>
+        <v>2542.0328234496</v>
       </c>
       <c r="U13" s="5">
-        <v>7966.03</v>
+        <v>2878.69</v>
       </c>
       <c r="V13" s="4">
-        <v>5265.40244146</v>
+        <v>1902.76227358</v>
       </c>
       <c r="W13" s="5">
-        <v>80734.5</v>
+        <v>24786.96</v>
       </c>
       <c r="X13" s="4">
-        <v>37675.8039735</v>
+        <v>11567.15711448</v>
       </c>
       <c r="Y13" s="4">
-        <v>59910.65219158</v>
+        <v>28209.0670882344</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="7">
-        <v>162.96</v>
-      </c>
-      <c r="C14" s="8">
-        <v>5235.50196288</v>
-      </c>
-      <c r="D14" s="7">
-        <v>12.96000000000001</v>
-      </c>
-      <c r="E14" s="8">
-        <v>832.7455257600004</v>
-      </c>
-      <c r="F14" s="9">
-        <v>7636.86</v>
-      </c>
-      <c r="G14" s="8">
-        <v>19386.80296938</v>
-      </c>
-      <c r="H14" s="9">
-        <v>75117</v>
-      </c>
-      <c r="I14" s="8">
-        <v>35054.324571</v>
-      </c>
-      <c r="J14" s="8">
-        <v>60509.37502902</v>
+      <c r="B14" s="11">
+        <v>172.7904</v>
+      </c>
+      <c r="C14" s="12">
+        <v>5551.3284141312</v>
+      </c>
+      <c r="D14" s="11">
+        <v>37.79040000000001</v>
+      </c>
+      <c r="E14" s="12">
+        <v>2428.2242682624</v>
+      </c>
+      <c r="F14" s="13">
+        <v>3204.74</v>
+      </c>
+      <c r="G14" s="12">
+        <v>8135.49848342</v>
+      </c>
+      <c r="H14" s="13">
+        <v>29647.92</v>
+      </c>
+      <c r="I14" s="12">
+        <v>13835.58729096</v>
+      </c>
+      <c r="J14" s="12">
+        <v>29950.63845677359</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="3">
-        <v>147.42</v>
+        <v>95.2512</v>
       </c>
       <c r="N14" s="4">
-        <v>11427.44719662</v>
+        <v>7383.5168797632</v>
       </c>
       <c r="O14" s="3">
-        <v>162.96</v>
+        <v>172.7904</v>
       </c>
       <c r="P14" s="4">
-        <v>5235.50196288</v>
+        <v>5551.3284141312</v>
       </c>
       <c r="Q14" s="3">
-        <v>0</v>
+        <v>10.2512</v>
       </c>
       <c r="R14" s="4">
-        <v>0</v>
+        <v>1589.2693895264</v>
       </c>
       <c r="S14" s="3">
-        <v>12.96000000000001</v>
+        <v>37.79040000000001</v>
       </c>
       <c r="T14" s="4">
-        <v>832.7455257600004</v>
+        <v>2428.2242682624</v>
       </c>
       <c r="U14" s="5">
-        <v>7636.86</v>
+        <v>3204.74</v>
       </c>
       <c r="V14" s="4">
-        <v>5047.82699652</v>
+        <v>2118.27545468</v>
       </c>
       <c r="W14" s="5">
-        <v>75117</v>
+        <v>29647.92</v>
       </c>
       <c r="X14" s="4">
-        <v>35054.324571</v>
+        <v>13835.58729096</v>
       </c>
       <c r="Y14" s="4">
-        <v>57597.84625278</v>
+        <v>32906.20169732319</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7">
-        <v>157.08</v>
-      </c>
-      <c r="C15" s="8">
-        <v>5046.59209824</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
-        <v>7389.16</v>
-      </c>
-      <c r="G15" s="8">
-        <v>18757.99596028</v>
-      </c>
-      <c r="H15" s="9">
-        <v>72586.5</v>
-      </c>
-      <c r="I15" s="8">
-        <v>33873.4338495</v>
-      </c>
-      <c r="J15" s="8">
-        <v>57678.02190802</v>
+      <c r="B15" s="11">
+        <v>160.9824</v>
+      </c>
+      <c r="C15" s="12">
+        <v>5171.9665635072</v>
+      </c>
+      <c r="D15" s="11">
+        <v>25.98240000000001</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1669.500567014401</v>
+      </c>
+      <c r="F15" s="13">
+        <v>2405.24</v>
+      </c>
+      <c r="G15" s="12">
+        <v>6105.901374919999</v>
+      </c>
+      <c r="H15" s="13">
+        <v>24285.12</v>
+      </c>
+      <c r="I15" s="12">
+        <v>11332.96695456</v>
+      </c>
+      <c r="J15" s="12">
+        <v>24280.3354600016</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M15" s="3">
-        <v>148.68</v>
+        <v>61.992</v>
       </c>
       <c r="N15" s="4">
-        <v>11525.11768548</v>
+        <v>6588.882185</v>
       </c>
       <c r="O15" s="3">
-        <v>157.08</v>
+        <v>160.9824</v>
       </c>
       <c r="P15" s="4">
-        <v>5046.59209824</v>
+        <v>5171.9665635072</v>
       </c>
       <c r="Q15" s="3">
         <v>0</v>
@@ -4362,89 +4535,79 @@
         <v>0</v>
       </c>
       <c r="S15" s="3">
-        <v>0</v>
+        <v>25.98240000000001</v>
       </c>
       <c r="T15" s="4">
-        <v>0</v>
+        <v>1669.500567014401</v>
       </c>
       <c r="U15" s="5">
-        <v>7389.16</v>
+        <v>2405.24</v>
       </c>
       <c r="V15" s="4">
-        <v>4884.101755119999</v>
+        <v>1589.82034568</v>
       </c>
       <c r="W15" s="5">
-        <v>72586.5</v>
+        <v>24285.12</v>
       </c>
       <c r="X15" s="4">
-        <v>33873.4338495</v>
+        <v>11332.96695456</v>
       </c>
       <c r="Y15" s="4">
-        <v>55329.24538833999</v>
+        <v>26353.1366157616</v>
       </c>
     </row>
     <row r="18" spans="13:18">
       <c r="M18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="13:18">
       <c r="M19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="10">
+        <v>41</v>
+      </c>
+      <c r="N19" s="14">
         <v>153</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R19" s="11">
-        <v>676679.25123173</v>
+        <v>45</v>
+      </c>
+      <c r="R19" s="15">
+        <v>231010.5726783288</v>
       </c>
     </row>
     <row r="20" spans="13:18">
       <c r="M20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N20" s="10">
+        <v>42</v>
+      </c>
+      <c r="N20" s="14">
         <v>153</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R20" s="11">
-        <v>653502.1838868</v>
+        <v>46</v>
+      </c>
+      <c r="R20" s="15">
+        <v>262756.9689998752</v>
       </c>
     </row>
     <row r="22" spans="13:18">
       <c r="M22" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="13:18">
-      <c r="M23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N23" s="10">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="13:18">
-      <c r="M24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N24" s="10">
-        <v>150</v>
-      </c>
+      <c r="M23" s="14">
+        <v>135</v>
+      </c>
+      <c r="N23" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="D1:E2"/>
@@ -4465,6 +4628,7 @@
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="Q18:R18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4474,13 +4638,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="0.140625" customWidth="1"/>
+    <col min="1" max="10" width="0.140625" customWidth="1"/>
     <col min="30" max="31" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4489,28 +4653,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
         <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -4518,28 +4682,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>140.28</v>
+        <v>101.1552</v>
       </c>
       <c r="C2">
-        <v>122.22</v>
+        <v>153</v>
       </c>
       <c r="D2">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E2">
-        <v>153</v>
-      </c>
-      <c r="F2">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G2">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="H2">
-        <v>157.5</v>
-      </c>
-      <c r="I2">
-        <v>152.25</v>
+        <v>119086.1570627712</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -4547,28 +4705,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>137.76</v>
+        <v>106.272</v>
       </c>
       <c r="C3">
-        <v>129.78</v>
+        <v>153</v>
       </c>
       <c r="D3">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E3">
-        <v>153</v>
-      </c>
-      <c r="F3">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G3">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="H3">
-        <v>157.5</v>
-      </c>
-      <c r="I3">
-        <v>152.25</v>
+        <v>115230.8537027712</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -4576,31 +4728,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>142.8</v>
+        <v>139.9248</v>
       </c>
       <c r="C4">
-        <v>127.26</v>
+        <v>153</v>
       </c>
       <c r="D4">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E4">
-        <v>153</v>
-      </c>
-      <c r="F4">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G4">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="H4">
-        <v>157.5</v>
-      </c>
-      <c r="I4">
-        <v>152.25</v>
+        <v>111375.5503427712</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE4" s="1"/>
     </row>
@@ -4609,69 +4755,49 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>136.08</v>
+        <v>134.6112</v>
       </c>
       <c r="C5">
-        <v>124.32</v>
+        <v>153</v>
       </c>
       <c r="D5">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E5">
-        <v>153</v>
-      </c>
-      <c r="F5">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G5">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="H5">
-        <v>157.5</v>
-      </c>
-      <c r="I5">
-        <v>152.25</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE5" s="10">
-        <v>145</v>
-      </c>
+        <v>107520.2469827712</v>
+      </c>
+      <c r="AD5" s="14">
+        <v>135</v>
+      </c>
+      <c r="AE5" s="14"/>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>138.6</v>
+        <v>135.2016</v>
       </c>
       <c r="C6">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="D6">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E6">
-        <v>153</v>
-      </c>
-      <c r="F6">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G6">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="H6">
-        <v>157.5</v>
-      </c>
-      <c r="I6">
-        <v>152.25</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE6" s="10">
-        <v>150</v>
+        <v>103664.9436227712</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -4679,123 +4805,99 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>132.72</v>
+        <v>103.5168</v>
       </c>
       <c r="C7">
-        <v>123.9</v>
+        <v>153</v>
       </c>
       <c r="D7">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E7">
-        <v>153</v>
-      </c>
-      <c r="F7">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G7">
-        <v>145</v>
+        <v>60</v>
       </c>
       <c r="H7">
-        <v>157.5</v>
-      </c>
-      <c r="I7">
-        <v>152.25</v>
-      </c>
+        <v>99809.64026277119</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE7" s="1"/>
     </row>
     <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>137.76</v>
+        <v>95.44799999999999</v>
       </c>
       <c r="C8">
-        <v>124.74</v>
+        <v>153</v>
       </c>
       <c r="D8">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E8">
-        <v>153</v>
-      </c>
-      <c r="F8">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G8">
-        <v>145</v>
+        <v>65</v>
       </c>
       <c r="H8">
-        <v>157.5</v>
-      </c>
-      <c r="I8">
-        <v>152.25</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE8" s="1"/>
+        <v>95818.8358406784</v>
+      </c>
+      <c r="AD8" s="16">
+        <v>92838.03440644077</v>
+      </c>
+      <c r="AE8" s="16"/>
     </row>
     <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>153.3</v>
+        <v>67.1088</v>
       </c>
       <c r="C9">
-        <v>151.62</v>
+        <v>153</v>
       </c>
       <c r="D9">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E9">
-        <v>153</v>
-      </c>
-      <c r="F9">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G9">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="H9">
-        <v>157.5</v>
-      </c>
-      <c r="I9">
-        <v>152.25</v>
-      </c>
-      <c r="AD9" s="12">
-        <v>6267.964864460024</v>
-      </c>
-      <c r="AE9" s="12"/>
+        <v>92377.69486963199</v>
+      </c>
     </row>
     <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>154.98</v>
+        <v>123.984</v>
       </c>
       <c r="C10">
-        <v>140.7</v>
+        <v>153</v>
       </c>
       <c r="D10">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E10">
-        <v>153</v>
-      </c>
-      <c r="F10">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G10">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="H10">
-        <v>157.5</v>
-      </c>
-      <c r="I10">
-        <v>152.25</v>
+        <v>89004.304429632</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -4803,28 +4905,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>157.5</v>
+        <v>174.5616</v>
       </c>
       <c r="C11">
-        <v>147.42</v>
+        <v>153</v>
       </c>
       <c r="D11">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E11">
-        <v>153</v>
-      </c>
-      <c r="F11">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G11">
-        <v>145</v>
+        <v>80</v>
       </c>
       <c r="H11">
-        <v>157.5</v>
-      </c>
-      <c r="I11">
-        <v>152.25</v>
+        <v>85630.913989632</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -4832,28 +4928,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>162.96</v>
+        <v>172.7904</v>
       </c>
       <c r="C12">
-        <v>147.42</v>
+        <v>153</v>
       </c>
       <c r="D12">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E12">
-        <v>153</v>
-      </c>
-      <c r="F12">
-        <v>150</v>
+        <v>141.75</v>
       </c>
       <c r="G12">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="H12">
-        <v>157.5</v>
-      </c>
-      <c r="I12">
-        <v>152.25</v>
+        <v>82257.52354963199</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -4861,40 +4951,298 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>157.08</v>
+        <v>160.9824</v>
       </c>
       <c r="C13">
-        <v>148.68</v>
+        <v>153</v>
       </c>
       <c r="D13">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E13">
-        <v>153</v>
-      </c>
-      <c r="F13">
+        <v>141.75</v>
+      </c>
+      <c r="G13">
+        <v>90</v>
+      </c>
+      <c r="H13">
+        <v>78884.13310963199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="G14">
+        <v>95</v>
+      </c>
+      <c r="H14">
+        <v>75481.95640454399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>72275.886130368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="G16">
+        <v>105</v>
+      </c>
+      <c r="H16">
+        <v>70116.40220832</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10">
+      <c r="G17">
+        <v>110</v>
+      </c>
+      <c r="H17">
+        <v>68629.79723270399</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10">
+      <c r="G18">
+        <v>115</v>
+      </c>
+      <c r="H18">
+        <v>67184.058472704</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19">
+        <v>120</v>
+      </c>
+      <c r="H19">
+        <v>65482.3275696</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10">
+      <c r="G20">
+        <v>125</v>
+      </c>
+      <c r="H20">
+        <v>64390.505658048</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10">
+      <c r="G21">
+        <v>130</v>
+      </c>
+      <c r="H21">
+        <v>62796.1578045312</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10">
+      <c r="G22">
+        <v>135</v>
+      </c>
+      <c r="H22">
+        <v>62170.9304076288</v>
+      </c>
+      <c r="J22">
+        <v>62170.9304076288</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10">
+      <c r="G23">
+        <v>140</v>
+      </c>
+      <c r="H23">
+        <v>62488.14476808959</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10">
+      <c r="G24">
+        <v>145</v>
+      </c>
+      <c r="H24">
+        <v>62970.0576880896</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10">
+      <c r="G25">
         <v>150</v>
       </c>
-      <c r="G13">
-        <v>145</v>
-      </c>
-      <c r="H13">
-        <v>157.5</v>
-      </c>
-      <c r="I13">
-        <v>152.25</v>
+      <c r="H25">
+        <v>63451.97060808959</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10">
+      <c r="G26">
+        <v>155</v>
+      </c>
+      <c r="H26">
+        <v>63549.48408107519</v>
+      </c>
+      <c r="I26">
+        <v>63549.48408107519</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10">
+      <c r="G27">
+        <v>160</v>
+      </c>
+      <c r="H27">
+        <v>64352.67228107519</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10">
+      <c r="G28">
+        <v>165</v>
+      </c>
+      <c r="H28">
+        <v>64784.3634493056</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10">
+      <c r="G29">
+        <v>170</v>
+      </c>
+      <c r="H29">
+        <v>65776.35870585599</v>
+      </c>
+    </row>
+    <row r="30" spans="7:10">
+      <c r="G30">
+        <v>175</v>
+      </c>
+      <c r="H30">
+        <v>67467.8088</v>
+      </c>
+    </row>
+    <row r="31" spans="7:10">
+      <c r="G31">
+        <v>180</v>
+      </c>
+      <c r="H31">
+        <v>69395.46047999999</v>
+      </c>
+    </row>
+    <row r="32" spans="7:10">
+      <c r="G32">
+        <v>185</v>
+      </c>
+      <c r="H32">
+        <v>71323.11215999999</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8">
+      <c r="G33">
+        <v>190</v>
+      </c>
+      <c r="H33">
+        <v>73250.76384</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8">
+      <c r="G34">
+        <v>195</v>
+      </c>
+      <c r="H34">
+        <v>75178.41552</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8">
+      <c r="G35">
+        <v>200</v>
+      </c>
+      <c r="H35">
+        <v>77106.06719999999</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8">
+      <c r="G36">
+        <v>205</v>
+      </c>
+      <c r="H36">
+        <v>79033.71888</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8">
+      <c r="G37">
+        <v>210</v>
+      </c>
+      <c r="H37">
+        <v>80961.37056</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8">
+      <c r="G38">
+        <v>215</v>
+      </c>
+      <c r="H38">
+        <v>82889.02223999999</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8">
+      <c r="G39">
+        <v>220</v>
+      </c>
+      <c r="H39">
+        <v>84816.67391999999</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8">
+      <c r="G40">
+        <v>225</v>
+      </c>
+      <c r="H40">
+        <v>86744.3256</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8">
+      <c r="G41">
+        <v>230</v>
+      </c>
+      <c r="H41">
+        <v>88671.97727999999</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8">
+      <c r="G42">
+        <v>235</v>
+      </c>
+      <c r="H42">
+        <v>90599.62896</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8">
+      <c r="G43">
+        <v>240</v>
+      </c>
+      <c r="H43">
+        <v>92527.28064</v>
+      </c>
+    </row>
+    <row r="44" spans="7:8">
+      <c r="G44">
+        <v>245</v>
+      </c>
+      <c r="H44">
+        <v>94454.93231999999</v>
+      </c>
+    </row>
+    <row r="45" spans="7:8">
+      <c r="G45">
+        <v>250</v>
+      </c>
+      <c r="H45">
+        <v>96382.584</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AD7:AE7"/>
     <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AD9:AE9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Verificação da formatação dos arquivos enviados
</commit_message>
<xml_diff>
--- a/arquivos/Teste.xlsx
+++ b/arquivos/Teste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
   <si>
     <t>Mês</t>
   </si>
@@ -63,25 +63,16 @@
     <t>Demanda Registrada na Ponta</t>
   </si>
   <si>
-    <t>Custo da Demanda na Ponta</t>
-  </si>
-  <si>
     <t>Demanda Registrada Fora Ponta</t>
   </si>
   <si>
-    <t>Custo da Demanda Fora Ponta</t>
-  </si>
-  <si>
-    <t>Ultrapassagem Registrada na Ponta</t>
-  </si>
-  <si>
-    <t>Custo da Ultrapassagem na Ponta</t>
-  </si>
-  <si>
-    <t>Ultrapassagem Registrada Fora Ponta</t>
-  </si>
-  <si>
-    <t>Custo da Ultrapassagem Fora Ponta</t>
+    <t>Custo da Demanda</t>
+  </si>
+  <si>
+    <t>Ultrapassagem Registrada</t>
+  </si>
+  <si>
+    <t>Custo da Ultrapassagem</t>
   </si>
   <si>
     <t>Consumo na Ponta</t>
@@ -141,12 +132,6 @@
     <t>Demanda Contratada Atual</t>
   </si>
   <si>
-    <t>Ponta</t>
-  </si>
-  <si>
-    <t>Fora Ponta</t>
-  </si>
-  <si>
     <t>Demanda Contratada Recomendada</t>
   </si>
   <si>
@@ -162,7 +147,7 @@
     <t>Utilizada</t>
   </si>
   <si>
-    <t>Contratada - 153 kW</t>
+    <t>Contratada - 160 kW</t>
   </si>
   <si>
     <t>Proposta - 135 kW</t>
@@ -244,13 +229,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +425,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$O$2:$O$13</c:f>
+              <c:f>Geral!$L$2:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -497,7 +482,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$Q$2:$Q$13</c:f>
+              <c:f>Geral!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -670,45 +655,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$K$2:$K$13</c:f>
+              <c:f>Geral!$H$2:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>993.94507268</c:v>
+                  <c:v>3817.36880042</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>957.7496983599999</c:v>
+                  <c:v>3678.35599534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1329.71731886</c:v>
+                  <c:v>5106.94357859</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2035.83116982</c:v>
+                  <c:v>7818.86102583</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1507.54130632</c:v>
+                  <c:v>5789.898563080001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1694.8900444</c:v>
+                  <c:v>6509.4345286</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1182.95287558</c:v>
+                  <c:v>4543.27660927</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>729.03670672</c:v>
+                  <c:v>2799.95550568</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1929.59153296</c:v>
+                  <c:v>7410.834580240001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1902.76227358</c:v>
+                  <c:v>7307.79349627</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2118.27545468</c:v>
+                  <c:v>8135.49848342</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1589.82034568</c:v>
+                  <c:v>6105.901374919999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -727,7 +712,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$M$2:$M$13</c:f>
+              <c:f>Geral!$J$2:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -847,11 +832,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>P</c:v>
+            <c:v>Ultrapassagem</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="31859C"/>
+              <a:srgbClr val="8064A2"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -900,7 +885,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Geral!$G$2:$G$13</c:f>
+              <c:f>Geral!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -932,70 +917,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>935.6564234495999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>821.8478682624003</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>FP</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="8064A2"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:val>
-            <c:numRef>
-              <c:f>Geral!$I$2:$I$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1385.4418154496</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1271.6332602624</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>512.9095590144008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1445,7 +1373,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Contratada - 153 kW</c:v>
+                  <c:v>Contratada - 160 kW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1467,40 +1395,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>153</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1769,10 +1697,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Recomendação'!$G$2:$G$45</c:f>
+              <c:f>'Recomendação'!$G$2:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>35</c:v>
                 </c:pt>
@@ -1904,16 +1832,19 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>255</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$H$2:$H$45</c:f>
+              <c:f>'Recomendação'!$H$2:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>119086.1570627712</c:v>
                 </c:pt>
@@ -2045,6 +1976,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>96382.584</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>98310.23567999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2081,12 +2015,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$I$2:$I$45</c:f>
+              <c:f>'Recomendação'!$I$2:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
-                <c:pt idx="24">
-                  <c:v>63549.48408107519</c:v>
+                <c:ptCount val="45"/>
+                <c:pt idx="25">
+                  <c:v>64352.67228107519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2122,10 +2056,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Recomendação'!$J$2:$J$45</c:f>
+              <c:f>'Recomendação'!$J$2:$J$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="20">
                   <c:v>62170.9304076288</c:v>
                 </c:pt>
@@ -2433,7 +2367,7 @@
   <tableColumns count="5">
     <tableColumn id="1" name="Mês"/>
     <tableColumn id="2" name="Utilizada"/>
-    <tableColumn id="3" name="Contratada - 153 kW"/>
+    <tableColumn id="3" name="Contratada - 160 kW"/>
     <tableColumn id="4" name="Proposta - 135 kW"/>
     <tableColumn id="5" name="Proposta + Tolerância de 5%"/>
   </tableColumns>
@@ -2442,8 +2376,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="G1:J45" totalsRowShown="0">
-  <autoFilter ref="G1:J45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="G1:J46" totalsRowShown="0">
+  <autoFilter ref="G1:J46"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Demandas Contratadas"/>
     <tableColumn id="2" name="Custos Anuais"/>
@@ -2739,7 +2673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2748,7 +2682,7 @@
     <col min="2" max="17" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2791,702 +2725,576 @@
       <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>64.1568</v>
       </c>
-      <c r="C2" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="3">
         <v>101.1552</v>
       </c>
-      <c r="E2" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="D2" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
         <v>1503.74</v>
       </c>
-      <c r="K2" s="4">
-        <v>993.94507268</v>
-      </c>
-      <c r="L2" s="5">
+      <c r="H2" s="4">
+        <v>3817.36880042</v>
+      </c>
+      <c r="I2" s="5">
         <v>12226.2</v>
       </c>
-      <c r="M2" s="4">
+      <c r="J2" s="4">
         <v>5705.515170600001</v>
       </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>66.5184</v>
       </c>
-      <c r="C3" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
         <v>106.272</v>
       </c>
-      <c r="E3" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="D3" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
         <v>1448.98</v>
       </c>
-      <c r="K3" s="4">
-        <v>957.7496983599999</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="H3" s="4">
+        <v>3678.35599534</v>
+      </c>
+      <c r="I3" s="5">
         <v>11714.52</v>
       </c>
-      <c r="M3" s="4">
+      <c r="J3" s="4">
         <v>5466.73304676</v>
       </c>
-      <c r="N3" s="6">
+      <c r="K3" s="6">
         <v>6.49</v>
       </c>
-      <c r="O3" s="4">
+      <c r="L3" s="4">
         <v>2.3342583</v>
       </c>
-      <c r="P3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>77.1456</v>
       </c>
-      <c r="C4" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <v>139.9248</v>
       </c>
-      <c r="E4" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="D4" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
         <v>2011.73</v>
       </c>
-      <c r="K4" s="4">
-        <v>1329.71731886</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="H4" s="4">
+        <v>5106.94357859</v>
+      </c>
+      <c r="I4" s="5">
         <v>16004.76</v>
       </c>
-      <c r="M4" s="4">
+      <c r="J4" s="4">
         <v>7468.82931588</v>
       </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>84.624</v>
       </c>
-      <c r="C5" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="3">
         <v>134.6112</v>
       </c>
-      <c r="E5" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="D5" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
         <v>3080.01</v>
       </c>
-      <c r="K5" s="4">
-        <v>2035.83116982</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="H5" s="4">
+        <v>7818.86102583</v>
+      </c>
+      <c r="I5" s="5">
         <v>20742.72</v>
       </c>
-      <c r="M5" s="4">
+      <c r="J5" s="4">
         <v>9679.859943360001</v>
       </c>
-      <c r="N5" s="6">
+      <c r="K5" s="6">
         <v>19.68</v>
       </c>
-      <c r="O5" s="4">
+      <c r="L5" s="4">
         <v>7.078305599999999</v>
       </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>90.7248</v>
       </c>
-      <c r="C6" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="3">
         <v>135.2016</v>
       </c>
-      <c r="E6" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="D6" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
         <v>2280.76</v>
       </c>
-      <c r="K6" s="4">
-        <v>1507.54130632</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="H6" s="4">
+        <v>5789.898563080001</v>
+      </c>
+      <c r="I6" s="5">
         <v>17269.2</v>
       </c>
-      <c r="M6" s="4">
+      <c r="J6" s="4">
         <v>8058.8966796</v>
       </c>
-      <c r="N6" s="6">
+      <c r="K6" s="6">
         <v>7.18</v>
       </c>
-      <c r="O6" s="4">
+      <c r="L6" s="4">
         <v>2.5824306</v>
       </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>71.0448</v>
       </c>
-      <c r="C7" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="3">
         <v>103.5168</v>
       </c>
-      <c r="E7" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="D7" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
         <v>2564.2</v>
       </c>
-      <c r="K7" s="4">
-        <v>1694.8900444</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="H7" s="4">
+        <v>6509.4345286</v>
+      </c>
+      <c r="I7" s="5">
         <v>16855.92</v>
       </c>
-      <c r="M7" s="4">
+      <c r="J7" s="4">
         <v>7866.034194960001</v>
       </c>
-      <c r="N7" s="6">
+      <c r="K7" s="6">
         <v>4.28</v>
       </c>
-      <c r="O7" s="4">
+      <c r="L7" s="4">
         <v>1.5393876</v>
       </c>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>56.4816</v>
       </c>
-      <c r="C8" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="3">
         <v>95.44799999999999</v>
       </c>
-      <c r="E8" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="D8" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
         <v>1789.69</v>
       </c>
-      <c r="K8" s="4">
-        <v>1182.95287558</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="H8" s="4">
+        <v>4543.27660927</v>
+      </c>
+      <c r="I8" s="5">
         <v>12231.12</v>
       </c>
-      <c r="M8" s="4">
+      <c r="J8" s="4">
         <v>5707.811152560001</v>
       </c>
-      <c r="N8" s="6">
+      <c r="K8" s="6">
         <v>6.39</v>
       </c>
-      <c r="O8" s="4">
+      <c r="L8" s="4">
         <v>2.2982913</v>
       </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>49.7904</v>
       </c>
-      <c r="C9" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9" s="3">
         <v>67.1088</v>
       </c>
-      <c r="E9" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
+      <c r="D9" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
         <v>1102.96</v>
       </c>
-      <c r="K9" s="4">
-        <v>729.03670672</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="H9" s="4">
+        <v>2799.95550568</v>
+      </c>
+      <c r="I9" s="5">
         <v>8255.76</v>
       </c>
-      <c r="M9" s="4">
+      <c r="J9" s="4">
         <v>3852.65772888</v>
       </c>
-      <c r="N9" s="6">
+      <c r="K9" s="6">
         <v>38.91</v>
       </c>
-      <c r="O9" s="4">
+      <c r="L9" s="4">
         <v>13.9947597</v>
       </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>85.2144</v>
       </c>
-      <c r="C10" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="3">
         <v>123.984</v>
       </c>
-      <c r="E10" s="4">
-        <v>4915.511783999999</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="D10" s="4">
+        <v>5140.404479999999</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
         <v>2919.28</v>
       </c>
-      <c r="K10" s="4">
-        <v>1929.59153296</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="H10" s="4">
+        <v>7410.834580240001</v>
+      </c>
+      <c r="I10" s="5">
         <v>19871.88</v>
       </c>
-      <c r="M10" s="4">
+      <c r="J10" s="4">
         <v>9273.471136439999</v>
       </c>
-      <c r="N10" s="6">
+      <c r="K10" s="6">
         <v>11.11</v>
       </c>
-      <c r="O10" s="4">
+      <c r="L10" s="4">
         <v>3.9959337</v>
       </c>
-      <c r="P10" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>81.86879999999999</v>
       </c>
-      <c r="C11" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="3">
         <v>174.5616</v>
       </c>
-      <c r="E11" s="4">
+      <c r="D11" s="4">
         <v>5608.232691724799</v>
       </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>21.5616</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1385.4418154496</v>
-      </c>
-      <c r="J11" s="5">
+      <c r="E11" s="3">
+        <v>14.5616</v>
+      </c>
+      <c r="F11" s="4">
+        <v>935.6564234495999</v>
+      </c>
+      <c r="G11" s="5">
         <v>2878.69</v>
       </c>
-      <c r="K11" s="4">
-        <v>1902.76227358</v>
-      </c>
-      <c r="L11" s="5">
+      <c r="H11" s="4">
+        <v>7307.79349627</v>
+      </c>
+      <c r="I11" s="5">
         <v>24786.96</v>
       </c>
-      <c r="M11" s="4">
+      <c r="J11" s="4">
         <v>11567.15711448</v>
       </c>
-      <c r="N11" s="6">
+      <c r="K11" s="6">
         <v>4.92</v>
       </c>
-      <c r="O11" s="4">
+      <c r="L11" s="4">
         <v>1.7695764</v>
       </c>
-      <c r="P11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3">
         <v>95.2512</v>
       </c>
-      <c r="C12" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="3">
         <v>172.7904</v>
       </c>
-      <c r="E12" s="4">
+      <c r="D12" s="4">
         <v>5551.3284141312</v>
       </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>19.79040000000001</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1271.6332602624</v>
-      </c>
-      <c r="J12" s="5">
+      <c r="E12" s="3">
+        <v>12.79040000000001</v>
+      </c>
+      <c r="F12" s="4">
+        <v>821.8478682624003</v>
+      </c>
+      <c r="G12" s="5">
         <v>3204.74</v>
       </c>
-      <c r="K12" s="4">
-        <v>2118.27545468</v>
-      </c>
-      <c r="L12" s="5">
+      <c r="H12" s="4">
+        <v>8135.49848342</v>
+      </c>
+      <c r="I12" s="5">
         <v>29647.92</v>
       </c>
-      <c r="M12" s="4">
+      <c r="J12" s="4">
         <v>13835.58729096</v>
       </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>61.992</v>
       </c>
-      <c r="C13" s="4">
-        <v>11859.987933</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="3">
         <v>160.9824</v>
       </c>
-      <c r="E13" s="4">
+      <c r="D13" s="4">
         <v>5171.9665635072</v>
       </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>7.982400000000013</v>
-      </c>
-      <c r="I13" s="4">
-        <v>512.9095590144008</v>
-      </c>
-      <c r="J13" s="5">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
         <v>2405.24</v>
       </c>
-      <c r="K13" s="4">
-        <v>1589.82034568</v>
-      </c>
-      <c r="L13" s="5">
+      <c r="H13" s="4">
+        <v>6105.901374919999</v>
+      </c>
+      <c r="I13" s="5">
         <v>24285.12</v>
       </c>
-      <c r="M13" s="4">
+      <c r="J13" s="4">
         <v>11332.96695456</v>
       </c>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="7">
         <v>884.8127999999999</v>
       </c>
-      <c r="C14" s="8">
-        <v>142319.855196</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C14" s="7">
         <v>1515.5568</v>
       </c>
-      <c r="E14" s="8">
-        <v>60571.13372536319</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7">
-        <v>49.33440000000002</v>
-      </c>
-      <c r="I14" s="8">
-        <v>3169.984634726401</v>
-      </c>
-      <c r="J14" s="9">
+      <c r="D14" s="8">
+        <v>62595.1679893632</v>
+      </c>
+      <c r="E14" s="7">
+        <v>27.352</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1757.504291712</v>
+      </c>
+      <c r="G14" s="9">
         <v>27190.02</v>
       </c>
-      <c r="K14" s="8">
-        <v>17972.11379964</v>
-      </c>
-      <c r="L14" s="9">
+      <c r="H14" s="8">
+        <v>69024.12254166001</v>
+      </c>
+      <c r="I14" s="9">
         <v>213892.08</v>
       </c>
-      <c r="M14" s="8">
+      <c r="J14" s="8">
         <v>99815.51972904</v>
       </c>
-      <c r="N14" s="10">
+      <c r="K14" s="10">
         <v>98.95999999999999</v>
       </c>
-      <c r="O14" s="8">
+      <c r="L14" s="8">
         <v>35.59294319999999</v>
       </c>
-      <c r="P14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
+      <c r="M14" s="7">
+        <v>0</v>
+      </c>
+      <c r="N14" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3512,48 +3320,48 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3563,37 +3371,37 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -3601,144 +3409,144 @@
     <row r="3" spans="1:25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="3">
         <v>101.1552</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
-        <v>0</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>1503.74</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="4">
         <v>3817.36880042</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="5">
         <v>12226.2</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="4">
         <v>5705.515170600001</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="4">
         <v>13860.10025102</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="11">
         <v>64.1568</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="11">
         <v>101.1552</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="4">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0</v>
-      </c>
-      <c r="T4" s="4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
+      <c r="Q4" s="11">
+        <v>0</v>
+      </c>
+      <c r="R4" s="12">
+        <v>0</v>
+      </c>
+      <c r="S4" s="11">
+        <v>0</v>
+      </c>
+      <c r="T4" s="12">
+        <v>0</v>
+      </c>
+      <c r="U4" s="13">
         <v>1503.74</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="12">
         <v>993.94507268</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="13">
         <v>12226.2</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="12">
         <v>5705.515170600001</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y4" s="12">
         <v>17625.55870828</v>
       </c>
     </row>
@@ -3746,73 +3554,73 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="3">
         <v>106.272</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
         <v>1448.98</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="4">
         <v>3678.35599534</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="5">
         <v>11714.52</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="4">
         <v>5466.73304676</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="4">
         <v>13482.3053221</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="11">
         <v>66.5184</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="11">
         <v>106.272</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="4">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
-      <c r="T5" s="4">
-        <v>0</v>
-      </c>
-      <c r="U5" s="5">
+      <c r="Q5" s="11">
+        <v>0</v>
+      </c>
+      <c r="R5" s="12">
+        <v>0</v>
+      </c>
+      <c r="S5" s="11">
+        <v>0</v>
+      </c>
+      <c r="T5" s="12">
+        <v>0</v>
+      </c>
+      <c r="U5" s="13">
         <v>1448.98</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="12">
         <v>957.7496983599999</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5" s="13">
         <v>11714.52</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5" s="12">
         <v>5466.73304676</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="12">
         <v>17350.58121012</v>
       </c>
     </row>
@@ -3820,73 +3628,73 @@
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="3">
         <v>139.9248</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="4">
         <v>4495.4379298944</v>
       </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
         <v>2011.73</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="4">
         <v>5106.94357859</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="5">
         <v>16004.76</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="4">
         <v>7468.82931588</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="4">
         <v>17071.2108243644</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="11">
         <v>77.1456</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="11">
         <v>139.9248</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="12">
         <v>4495.4379298944</v>
       </c>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="4">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="T6" s="4">
-        <v>0</v>
-      </c>
-      <c r="U6" s="5">
+      <c r="Q6" s="11">
+        <v>0</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0</v>
+      </c>
+      <c r="S6" s="11">
+        <v>0</v>
+      </c>
+      <c r="T6" s="12">
+        <v>0</v>
+      </c>
+      <c r="U6" s="13">
         <v>2011.73</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="12">
         <v>1329.71731886</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="13">
         <v>16004.76</v>
       </c>
-      <c r="X6" s="4">
+      <c r="X6" s="12">
         <v>7468.82931588</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="12">
         <v>19882.8667496344</v>
       </c>
     </row>
@@ -3894,73 +3702,73 @@
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="3">
         <v>134.6112</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
         <v>3080.01</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="4">
         <v>7818.86102583</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="5">
         <v>20742.72</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="4">
         <v>9679.859943360001</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="4">
         <v>21835.93724919</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="11">
         <v>84.624</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="11">
         <v>134.6112</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q7" s="3">
-        <v>0</v>
-      </c>
-      <c r="R7" s="4">
-        <v>0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4">
-        <v>0</v>
-      </c>
-      <c r="U7" s="5">
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0</v>
+      </c>
+      <c r="S7" s="11">
+        <v>0</v>
+      </c>
+      <c r="T7" s="12">
+        <v>0</v>
+      </c>
+      <c r="U7" s="13">
         <v>3080.01</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="12">
         <v>2035.83116982</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="13">
         <v>20742.72</v>
       </c>
-      <c r="X7" s="4">
+      <c r="X7" s="12">
         <v>9679.859943360001</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="12">
         <v>22641.78957818</v>
       </c>
     </row>
@@ -3968,73 +3776,73 @@
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="3">
         <v>135.2016</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="4">
         <v>4343.6931896448</v>
       </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
         <v>2280.76</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="4">
         <v>5789.898563080001</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="5">
         <v>17269.2</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="4">
         <v>8058.8966796</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="4">
         <v>18192.4884323248</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="11">
         <v>90.7248</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="12">
         <v>7032.6472759728</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="11">
         <v>135.2016</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="12">
         <v>4343.6931896448</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="11">
         <v>5.724800000000002</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="12">
         <v>887.5301819456002</v>
       </c>
-      <c r="S8" s="3">
-        <v>0</v>
-      </c>
-      <c r="T8" s="4">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5">
+      <c r="S8" s="11">
+        <v>0</v>
+      </c>
+      <c r="T8" s="12">
+        <v>0</v>
+      </c>
+      <c r="U8" s="13">
         <v>2280.76</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="12">
         <v>1507.54130632</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8" s="13">
         <v>17269.2</v>
       </c>
-      <c r="X8" s="4">
+      <c r="X8" s="12">
         <v>8058.8966796</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Y8" s="12">
         <v>21830.3086334832</v>
       </c>
     </row>
@@ -4042,73 +3850,73 @@
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="3">
         <v>103.5168</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
         <v>2564.2</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="4">
         <v>6509.4345286</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="5">
         <v>16855.92</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="4">
         <v>7866.034194960001</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="4">
         <v>18712.68500356</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="11">
         <v>71.0448</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="11">
         <v>103.5168</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
-      <c r="R9" s="4">
-        <v>0</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
-      <c r="T9" s="4">
-        <v>0</v>
-      </c>
-      <c r="U9" s="5">
+      <c r="Q9" s="11">
+        <v>0</v>
+      </c>
+      <c r="R9" s="12">
+        <v>0</v>
+      </c>
+      <c r="S9" s="11">
+        <v>0</v>
+      </c>
+      <c r="T9" s="12">
+        <v>0</v>
+      </c>
+      <c r="U9" s="13">
         <v>2564.2</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="12">
         <v>1694.8900444</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9" s="13">
         <v>16855.92</v>
       </c>
-      <c r="X9" s="4">
+      <c r="X9" s="12">
         <v>7866.034194960001</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="12">
         <v>20487.02270436</v>
       </c>
     </row>
@@ -4116,73 +3924,73 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="3">
         <v>95.44799999999999</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12">
-        <v>0</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
         <v>1789.69</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="4">
         <v>4543.27660927</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="5">
         <v>12231.12</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="4">
         <v>5707.811152560001</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="4">
         <v>14588.30404183</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="11">
         <v>56.4816</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="11">
         <v>95.44799999999999</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q10" s="3">
-        <v>0</v>
-      </c>
-      <c r="R10" s="4">
-        <v>0</v>
-      </c>
-      <c r="S10" s="3">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5">
+      <c r="Q10" s="11">
+        <v>0</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0</v>
+      </c>
+      <c r="S10" s="11">
+        <v>0</v>
+      </c>
+      <c r="T10" s="12">
+        <v>0</v>
+      </c>
+      <c r="U10" s="13">
         <v>1789.69</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="12">
         <v>1182.95287558</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="13">
         <v>12231.12</v>
       </c>
-      <c r="X10" s="4">
+      <c r="X10" s="12">
         <v>5707.811152560001</v>
       </c>
-      <c r="Y10" s="4">
+      <c r="Y10" s="12">
         <v>17816.86249314</v>
       </c>
     </row>
@@ -4190,73 +3998,73 @@
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="3">
         <v>67.1088</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
         <v>1102.96</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="4">
         <v>2799.95550568</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="5">
         <v>8255.76</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="4">
         <v>3852.65772888</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="4">
         <v>10989.82951456</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="11">
         <v>49.7904</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="11">
         <v>67.1088</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="4">
-        <v>0</v>
-      </c>
-      <c r="S11" s="3">
-        <v>0</v>
-      </c>
-      <c r="T11" s="4">
-        <v>0</v>
-      </c>
-      <c r="U11" s="5">
+      <c r="Q11" s="11">
+        <v>0</v>
+      </c>
+      <c r="R11" s="12">
+        <v>0</v>
+      </c>
+      <c r="S11" s="11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="12">
+        <v>0</v>
+      </c>
+      <c r="U11" s="13">
         <v>1102.96</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11" s="12">
         <v>729.03670672</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11" s="13">
         <v>8255.76</v>
       </c>
-      <c r="X11" s="4">
+      <c r="X11" s="12">
         <v>3852.65772888</v>
       </c>
-      <c r="Y11" s="4">
+      <c r="Y11" s="12">
         <v>15507.7929006</v>
       </c>
     </row>
@@ -4264,73 +4072,73 @@
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="3">
         <v>123.984</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="4">
         <v>4337.21628</v>
       </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="13">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
         <v>2919.28</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="4">
         <v>7410.834580240001</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="5">
         <v>19871.88</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="4">
         <v>9273.471136439999</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="4">
         <v>21021.52199668</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="11">
         <v>85.2144</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="12">
         <v>6605.5016713584</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="11">
         <v>123.984</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="12">
         <v>4337.21628</v>
       </c>
-      <c r="Q12" s="3">
-        <v>0</v>
-      </c>
-      <c r="R12" s="4">
-        <v>0</v>
-      </c>
-      <c r="S12" s="3">
-        <v>0</v>
-      </c>
-      <c r="T12" s="4">
-        <v>0</v>
-      </c>
-      <c r="U12" s="5">
+      <c r="Q12" s="11">
+        <v>0</v>
+      </c>
+      <c r="R12" s="12">
+        <v>0</v>
+      </c>
+      <c r="S12" s="11">
+        <v>0</v>
+      </c>
+      <c r="T12" s="12">
+        <v>0</v>
+      </c>
+      <c r="U12" s="13">
         <v>2919.28</v>
       </c>
-      <c r="V12" s="4">
+      <c r="V12" s="12">
         <v>1929.59153296</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="13">
         <v>19871.88</v>
       </c>
-      <c r="X12" s="4">
+      <c r="X12" s="12">
         <v>9273.471136439999</v>
       </c>
-      <c r="Y12" s="4">
+      <c r="Y12" s="12">
         <v>22145.7806207584</v>
       </c>
     </row>
@@ -4338,73 +4146,73 @@
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="3">
         <v>174.5616</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="4">
         <v>5608.232691724799</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="3">
         <v>39.5616</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="4">
         <v>2542.0328234496</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="5">
         <v>2878.69</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="4">
         <v>7307.79349627</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="5">
         <v>24786.96</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="4">
         <v>11567.15711448</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="4">
         <v>27025.2161259244</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="11">
         <v>81.86879999999999</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="11">
         <v>174.5616</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="12">
         <v>5608.232691724799</v>
       </c>
-      <c r="Q13" s="3">
-        <v>0</v>
-      </c>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-      <c r="S13" s="3">
+      <c r="Q13" s="11">
+        <v>0</v>
+      </c>
+      <c r="R13" s="12">
+        <v>0</v>
+      </c>
+      <c r="S13" s="11">
         <v>39.5616</v>
       </c>
-      <c r="T13" s="4">
+      <c r="T13" s="12">
         <v>2542.0328234496</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="13">
         <v>2878.69</v>
       </c>
-      <c r="V13" s="4">
+      <c r="V13" s="12">
         <v>1902.76227358</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="13">
         <v>24786.96</v>
       </c>
-      <c r="X13" s="4">
+      <c r="X13" s="12">
         <v>11567.15711448</v>
       </c>
-      <c r="Y13" s="4">
+      <c r="Y13" s="12">
         <v>28209.0670882344</v>
       </c>
     </row>
@@ -4412,73 +4220,73 @@
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="3">
         <v>172.7904</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="4">
         <v>5551.3284141312</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="3">
         <v>37.79040000000001</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="4">
         <v>2428.2242682624</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="5">
         <v>3204.74</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="4">
         <v>8135.49848342</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="5">
         <v>29647.92</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="4">
         <v>13835.58729096</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="4">
         <v>29950.63845677359</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="11">
         <v>95.2512</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="12">
         <v>7383.5168797632</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="11">
         <v>172.7904</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="12">
         <v>5551.3284141312</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="11">
         <v>10.2512</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R14" s="12">
         <v>1589.2693895264</v>
       </c>
-      <c r="S14" s="3">
+      <c r="S14" s="11">
         <v>37.79040000000001</v>
       </c>
-      <c r="T14" s="4">
+      <c r="T14" s="12">
         <v>2428.2242682624</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="13">
         <v>3204.74</v>
       </c>
-      <c r="V14" s="4">
+      <c r="V14" s="12">
         <v>2118.27545468</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14" s="13">
         <v>29647.92</v>
       </c>
-      <c r="X14" s="4">
+      <c r="X14" s="12">
         <v>13835.58729096</v>
       </c>
-      <c r="Y14" s="4">
+      <c r="Y14" s="12">
         <v>32906.20169732319</v>
       </c>
     </row>
@@ -4486,109 +4294,101 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="3">
         <v>160.9824</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="4">
         <v>5171.9665635072</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="3">
         <v>25.98240000000001</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="4">
         <v>1669.500567014401</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="5">
         <v>2405.24</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="4">
         <v>6105.901374919999</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="5">
         <v>24285.12</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="4">
         <v>11332.96695456</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="4">
         <v>24280.3354600016</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="11">
         <v>61.992</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="12">
         <v>6588.882185</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="11">
         <v>160.9824</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="12">
         <v>5171.9665635072</v>
       </c>
-      <c r="Q15" s="3">
-        <v>0</v>
-      </c>
-      <c r="R15" s="4">
-        <v>0</v>
-      </c>
-      <c r="S15" s="3">
+      <c r="Q15" s="11">
+        <v>0</v>
+      </c>
+      <c r="R15" s="12">
+        <v>0</v>
+      </c>
+      <c r="S15" s="11">
         <v>25.98240000000001</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" s="12">
         <v>1669.500567014401</v>
       </c>
-      <c r="U15" s="5">
+      <c r="U15" s="13">
         <v>2405.24</v>
       </c>
-      <c r="V15" s="4">
+      <c r="V15" s="12">
         <v>1589.82034568</v>
       </c>
-      <c r="W15" s="5">
+      <c r="W15" s="13">
         <v>24285.12</v>
       </c>
-      <c r="X15" s="4">
+      <c r="X15" s="12">
         <v>11332.96695456</v>
       </c>
-      <c r="Y15" s="4">
+      <c r="Y15" s="12">
         <v>26353.1366157616</v>
       </c>
     </row>
     <row r="18" spans="13:18">
       <c r="M18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="13:18">
-      <c r="M19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N19" s="14">
-        <v>153</v>
-      </c>
+      <c r="M19" s="14">
+        <v>160</v>
+      </c>
+      <c r="N19" s="14"/>
       <c r="Q19" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="R19" s="15">
         <v>231010.5726783288</v>
       </c>
     </row>
     <row r="20" spans="13:18">
-      <c r="M20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N20" s="14">
-        <v>153</v>
-      </c>
       <c r="Q20" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="R20" s="15">
         <v>262756.9689998752</v>
@@ -4596,7 +4396,7 @@
     </row>
     <row r="22" spans="13:18">
       <c r="M22" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N22" s="1"/>
     </row>
@@ -4607,7 +4407,7 @@
       <c r="N23" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="D1:E2"/>
@@ -4627,6 +4427,7 @@
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="Q18:R18"/>
@@ -4638,7 +4439,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4653,28 +4454,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -4685,7 +4486,7 @@
         <v>101.1552</v>
       </c>
       <c r="C2">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D2">
         <v>135</v>
@@ -4708,7 +4509,7 @@
         <v>106.272</v>
       </c>
       <c r="C3">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D3">
         <v>135</v>
@@ -4731,7 +4532,7 @@
         <v>139.9248</v>
       </c>
       <c r="C4">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D4">
         <v>135</v>
@@ -4746,7 +4547,7 @@
         <v>111375.5503427712</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="AE4" s="1"/>
     </row>
@@ -4758,7 +4559,7 @@
         <v>134.6112</v>
       </c>
       <c r="C5">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D5">
         <v>135</v>
@@ -4785,7 +4586,7 @@
         <v>135.2016</v>
       </c>
       <c r="C6">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D6">
         <v>135</v>
@@ -4808,7 +4609,7 @@
         <v>103.5168</v>
       </c>
       <c r="C7">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D7">
         <v>135</v>
@@ -4823,7 +4624,7 @@
         <v>99809.64026277119</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="AE7" s="1"/>
     </row>
@@ -4835,7 +4636,7 @@
         <v>95.44799999999999</v>
       </c>
       <c r="C8">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D8">
         <v>135</v>
@@ -4850,7 +4651,7 @@
         <v>95818.8358406784</v>
       </c>
       <c r="AD8" s="16">
-        <v>92838.03440644077</v>
+        <v>2181.741873446357</v>
       </c>
       <c r="AE8" s="16"/>
     </row>
@@ -4862,7 +4663,7 @@
         <v>67.1088</v>
       </c>
       <c r="C9">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D9">
         <v>135</v>
@@ -4885,7 +4686,7 @@
         <v>123.984</v>
       </c>
       <c r="C10">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D10">
         <v>135</v>
@@ -4908,7 +4709,7 @@
         <v>174.5616</v>
       </c>
       <c r="C11">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D11">
         <v>135</v>
@@ -4931,7 +4732,7 @@
         <v>172.7904</v>
       </c>
       <c r="C12">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D12">
         <v>135</v>
@@ -4954,7 +4755,7 @@
         <v>160.9824</v>
       </c>
       <c r="C13">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D13">
         <v>135</v>
@@ -5075,9 +4876,6 @@
       <c r="H26">
         <v>63549.48408107519</v>
       </c>
-      <c r="I26">
-        <v>63549.48408107519</v>
-      </c>
     </row>
     <row r="27" spans="7:10">
       <c r="G27">
@@ -5086,6 +4884,9 @@
       <c r="H27">
         <v>64352.67228107519</v>
       </c>
+      <c r="I27">
+        <v>64352.67228107519</v>
+      </c>
     </row>
     <row r="28" spans="7:10">
       <c r="G28">
@@ -5229,6 +5030,14 @@
       </c>
       <c r="H45">
         <v>96382.584</v>
+      </c>
+    </row>
+    <row r="46" spans="7:8">
+      <c r="G46">
+        <v>255</v>
+      </c>
+      <c r="H46">
+        <v>98310.23567999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>